<commit_message>
correction of sensitivity analysis
</commit_message>
<xml_diff>
--- a/CBA (3).xlsx
+++ b/CBA (3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanelmaheinonen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a630b34756993743/Desktop/ETHZ/Transport Planning Methods/TransportPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60C97A6-90D9-F948-ACE4-80043545B60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{B60C97A6-90D9-F948-ACE4-80043545B60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F29F5F7-B2EB-4507-BDC2-5AFE9F4893D1}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="28520" windowHeight="16580" activeTab="1" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tunnel" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -309,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
   <si>
     <t>Weekly benefits</t>
   </si>
@@ -723,9 +720,6 @@
     <t>Building Costs</t>
   </si>
   <si>
-    <t>Even if costs are twice what they are projected, still higher benefits than costs</t>
-  </si>
-  <si>
     <t>Discount Rate</t>
   </si>
   <si>
@@ -764,7 +758,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0\ [$CHF-100C]_-;\-* #,##0\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="179" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -947,7 +941,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1027,13 +1021,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -1052,6 +1043,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1353,30 +1348,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083A40F-175A-4EEC-B4D7-09BE1D9F546C}">
   <dimension ref="A1:R134"/>
   <sheetViews>
-    <sheetView topLeftCell="D26" zoomScale="106" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="47.5" customWidth="1"/>
-    <col min="5" max="5" width="5.5" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="11" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" customWidth="1"/>
+    <col min="4" max="4" width="47.453125" customWidth="1"/>
+    <col min="5" max="5" width="5.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.36328125" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" customWidth="1"/>
+    <col min="10" max="11" width="17.453125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" customWidth="1"/>
+    <col min="17" max="17" width="11.36328125" customWidth="1"/>
+    <col min="18" max="18" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>43</v>
       </c>
@@ -1384,7 +1379,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1395,13 +1390,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C4" s="1"/>
       <c r="G4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1425,7 +1420,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1440,7 +1435,7 @@
         <v>65000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>320000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1470,7 +1465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -1485,7 +1480,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
@@ -1500,7 +1495,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -1515,7 +1510,7 @@
         <v>4200000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G12" t="s">
         <v>40</v>
       </c>
@@ -1523,7 +1518,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="G13" t="s">
@@ -1535,13 +1530,13 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B15" s="11" t="s">
         <v>25</v>
       </c>
@@ -1559,7 +1554,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C16" s="9" t="s">
         <v>28</v>
       </c>
@@ -1574,7 +1569,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1583,14 +1578,14 @@
         <v>71710187.283656985</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="G18" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
@@ -1609,7 +1604,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
@@ -1625,7 +1620,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="G21" t="s">
@@ -1635,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="28" t="s">
         <v>81</v>
       </c>
@@ -1652,7 +1647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
       <c r="D23" s="5"/>
       <c r="F23" s="6"/>
@@ -1666,7 +1661,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="5"/>
       <c r="F24" s="6"/>
@@ -1677,7 +1672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>95</v>
       </c>
@@ -1696,7 +1691,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -1717,7 +1712,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="34" t="s">
         <v>45</v>
@@ -1736,7 +1731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="34" t="s">
         <v>6</v>
@@ -1751,7 +1746,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="34" t="s">
         <v>5</v>
@@ -1770,7 +1765,7 @@
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="34" t="s">
         <v>49</v>
@@ -1791,7 +1786,7 @@
         <v>1240000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
@@ -1814,17 +1809,17 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="5"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="5"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
       <c r="D34" s="3"/>
       <c r="F34" s="6"/>
@@ -1836,7 +1831,7 @@
       </c>
       <c r="K34" s="33"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C35" s="1"/>
       <c r="D35" s="5"/>
       <c r="F35" s="6"/>
@@ -1858,7 +1853,7 @@
       </c>
       <c r="R35" s="22"/>
     </row>
-    <row r="36" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C36" s="35" t="s">
         <v>97</v>
       </c>
@@ -1902,7 +1897,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +1955,7 @@
         <v>12.899999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="48" t="s">
         <v>8</v>
       </c>
@@ -2013,7 +2008,7 @@
       </c>
       <c r="R38" s="19"/>
     </row>
-    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B39" s="34" t="s">
         <v>63</v>
       </c>
@@ -2055,7 +2050,7 @@
       </c>
       <c r="R39" s="19"/>
     </row>
-    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D40" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2090,7 +2085,7 @@
       </c>
       <c r="R40" s="19"/>
     </row>
-    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B41" s="36" t="s">
         <v>49</v>
       </c>
@@ -2104,10 +2099,10 @@
       </c>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>89</v>
       </c>
@@ -2120,10 +2115,10 @@
         <v>63862565.4354067</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="27" t="s">
         <v>75</v>
       </c>
@@ -2133,7 +2128,7 @@
         <v>2353376160.1742077</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="41" t="s">
         <v>15</v>
       </c>
@@ -2142,12 +2137,12 @@
         <v>1.1601565562363165</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -2158,169 +2153,158 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B52" s="50">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B52" s="49">
         <v>1</v>
       </c>
-      <c r="C52" s="26">
-        <f>B52*$D$22</f>
+      <c r="C52" s="2">
         <v>2028498781.0686817</v>
       </c>
-      <c r="D52" s="52">
+      <c r="D52" s="51">
         <f>B48</f>
         <v>1.1601565562363165</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="50">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B53" s="49">
         <v>0.5</v>
       </c>
-      <c r="C53" s="26">
-        <f t="shared" ref="C53:C56" si="2">B53*$D$22</f>
+      <c r="C53" s="2">
         <v>1014249390.5343409</v>
       </c>
-      <c r="D53" s="52">
+      <c r="D53" s="51">
         <f t="dataTable" ref="D53:D56" dt2D="0" dtr="0" r1="D22" ca="1"/>
         <v>2.3203131124726331</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="50">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B54" s="49">
         <v>0.75</v>
       </c>
-      <c r="C54" s="26">
-        <f t="shared" si="2"/>
+      <c r="C54" s="2">
         <v>1521374085.8015113</v>
       </c>
-      <c r="D54" s="52">
-        <v>3.0937508166301777</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B55" s="50">
+      <c r="D54" s="51">
+        <v>1.5468754083150889</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B55" s="49">
         <v>1.5</v>
       </c>
-      <c r="C55" s="26">
-        <f t="shared" si="2"/>
+      <c r="C55" s="2">
         <v>3042748171.6030226</v>
       </c>
-      <c r="D55" s="52">
-        <v>2.0625005444201188</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B56" s="50">
+      <c r="D55" s="51">
+        <v>0.77343770415754443</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B56" s="49">
         <v>2</v>
       </c>
-      <c r="C56" s="26">
-        <f t="shared" si="2"/>
+      <c r="C56" s="2">
         <v>4056997562.1373634</v>
       </c>
-      <c r="D56" s="52">
-        <v>1.0312502722100594</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="D56" s="51">
+        <v>0.58007827811815826</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" s="54"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B58" s="56">
+        <v>128</v>
+      </c>
+      <c r="B58" s="53">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C58" s="52">
+      <c r="C58" s="51">
         <f>B48</f>
         <v>1.1601565562363165</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="C59" s="51">
+        <f t="dataTable" ref="C59:C61" dt2D="0" dtr="0" r1="H13" ca="1"/>
+        <v>0.71054629453694962</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="B59" s="56">
-        <v>0.05</v>
-      </c>
-      <c r="C59" s="52">
-        <f t="dataTable" ref="C59:C62" dt2D="0" dtr="0" r1="H13" ca="1"/>
-        <v>0.71054629453694962</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="B60" s="45">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C60" s="52">
+      <c r="C60" s="51">
         <v>0.52847290598642149</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B61" s="56">
+        <v>127</v>
+      </c>
+      <c r="B61" s="53">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C61" s="52">
+      <c r="C61" s="51">
         <v>1.4766559831584645</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
       <c r="B62" s="23"/>
-      <c r="C62" s="52">
-        <v>2.2330329535056106</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C62" s="51"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" t="s">
         <v>132</v>
       </c>
-      <c r="C64" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B65">
         <f>H38</f>
         <v>14.4</v>
       </c>
-      <c r="C65" s="55">
+      <c r="C65" s="52">
         <f>B48</f>
         <v>1.1601565562363165</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B66">
         <v>20.8</v>
       </c>
-      <c r="C66" s="55">
-        <f t="dataTable" ref="C66" dt2D="0" dtr="0" r1="H38" ca="1"/>
+      <c r="C66" s="52">
+        <f t="dataTable" ref="C66" dt2D="0" dtr="0" r1="H38"/>
         <v>1.6638881136021531</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -2329,7 +2313,7 @@
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -2338,7 +2322,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2346,610 +2330,610 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>0</v>
       </c>
       <c r="B74" s="26">
-        <f>$D$43*(1+$B$72)^-A74*(1+$B$71)^A74</f>
+        <f t="shared" ref="B74:B105" si="2">$D$43*(1+$B$72)^-A74*(1+$B$71)^A74</f>
         <v>63862565.4354067</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
       <c r="B75" s="26">
-        <f>$D$43*(1+$B$72)^-A75*(1+$B$71)^A75</f>
+        <f t="shared" si="2"/>
         <v>62688117.280814111</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2</v>
       </c>
       <c r="B76" s="26">
-        <f>$D$43*(1+$B$72)^-A76*(1+$B$71)^A76</f>
+        <f t="shared" si="2"/>
         <v>61535267.514235236</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
         <f>A76+1</f>
         <v>3</v>
       </c>
       <c r="B77" s="26">
-        <f>$D$43*(1+$B$72)^-A77*(1+$B$71)^A77</f>
+        <f t="shared" si="2"/>
         <v>60403618.936046623</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" ref="A78:A134" si="3">A77+1</f>
         <v>4</v>
       </c>
       <c r="B78" s="26">
-        <f>$D$43*(1+$B$72)^-A78*(1+$B$71)^A78</f>
+        <f t="shared" si="2"/>
         <v>59292781.651222758</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B79" s="26">
-        <f>$D$43*(1+$B$72)^-A79*(1+$B$71)^A79</f>
+        <f t="shared" si="2"/>
         <v>58202372.935002707</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B80" s="26">
-        <f>$D$43*(1+$B$72)^-A80*(1+$B$71)^A80</f>
+        <f t="shared" si="2"/>
         <v>57132017.101027302</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B81" s="26">
-        <f>$D$43*(1+$B$72)^-A81*(1+$B$71)^A81</f>
+        <f t="shared" si="2"/>
         <v>56081345.371901102</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B82" s="26">
-        <f>$D$43*(1+$B$72)^-A82*(1+$B$71)^A82</f>
+        <f t="shared" si="2"/>
         <v>55049995.752134927</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B83" s="26">
-        <f>$D$43*(1+$B$72)^-A83*(1+$B$71)^A83</f>
+        <f t="shared" si="2"/>
         <v>54037612.903424948</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B84" s="26">
-        <f>$D$43*(1+$B$72)^-A84*(1+$B$71)^A84</f>
+        <f t="shared" si="2"/>
         <v>53043848.02222538</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B85" s="26">
-        <f>$D$43*(1+$B$72)^-A85*(1+$B$71)^A85</f>
+        <f t="shared" si="2"/>
         <v>52068358.719572745</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B86" s="26">
-        <f>$D$43*(1+$B$72)^-A86*(1+$B$71)^A86</f>
+        <f t="shared" si="2"/>
         <v>51110808.903120138</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B87" s="26">
-        <f>$D$43*(1+$B$72)^-A87*(1+$B$71)^A87</f>
+        <f t="shared" si="2"/>
         <v>50170868.661340795</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B88" s="26">
-        <f>$D$43*(1+$B$72)^-A88*(1+$B$71)^A88</f>
+        <f t="shared" si="2"/>
         <v>49248214.149861522</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B89" s="26">
-        <f>$D$43*(1+$B$72)^-A89*(1+$B$71)^A89</f>
+        <f t="shared" si="2"/>
         <v>48342527.479886018</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90">
         <f>A89+1</f>
         <v>16</v>
       </c>
       <c r="B90" s="26">
-        <f>$D$43*(1+$B$72)^-A90*(1+$B$71)^A90</f>
+        <f t="shared" si="2"/>
         <v>47453496.608670563</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B91" s="26">
-        <f>$D$43*(1+$B$72)^-A91*(1+$B$71)^A91</f>
+        <f t="shared" si="2"/>
         <v>46580815.232013553</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B92" s="26">
-        <f>$D$43*(1+$B$72)^-A92*(1+$B$71)^A92</f>
+        <f t="shared" si="2"/>
         <v>45724182.678722374</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B93" s="26">
-        <f>$D$43*(1+$B$72)^-A93*(1+$B$71)^A93</f>
+        <f t="shared" si="2"/>
         <v>44883303.807020999</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B94" s="26">
-        <f>$D$43*(1+$B$72)^-A94*(1+$B$71)^A94</f>
+        <f t="shared" si="2"/>
         <v>44057888.902862623</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B95" s="26">
-        <f>$D$43*(1+$B$72)^-A95*(1+$B$71)^A95</f>
+        <f t="shared" si="2"/>
         <v>43247653.580112427</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B96" s="26">
-        <f>$D$43*(1+$B$72)^-A96*(1+$B$71)^A96</f>
+        <f t="shared" si="2"/>
         <v>42452318.682565972</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B97" s="26">
-        <f>$D$43*(1+$B$72)^-A97*(1+$B$71)^A97</f>
+        <f t="shared" si="2"/>
         <v>41671610.187769525</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B98" s="26">
-        <f>$D$43*(1+$B$72)^-A98*(1+$B$71)^A98</f>
+        <f t="shared" si="2"/>
         <v>40905259.112609081</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B99" s="26">
-        <f>$D$43*(1+$B$72)^-A99*(1+$B$71)^A99</f>
+        <f t="shared" si="2"/>
         <v>40153001.42063573</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B100" s="26">
-        <f>$D$43*(1+$B$72)^-A100*(1+$B$71)^A100</f>
+        <f t="shared" si="2"/>
         <v>39414577.93109528</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B101" s="26">
-        <f>$D$43*(1+$B$72)^-A101*(1+$B$71)^A101</f>
+        <f t="shared" si="2"/>
         <v>38689734.229630738</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B102" s="26">
-        <f>$D$43*(1+$B$72)^-A102*(1+$B$71)^A102</f>
+        <f t="shared" si="2"/>
         <v>37978220.5806273</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103">
         <f>A102+1</f>
         <v>29</v>
       </c>
       <c r="B103" s="26">
-        <f>$D$43*(1+$B$72)^-A103*(1+$B$71)^A103</f>
+        <f t="shared" si="2"/>
         <v>37279791.841168925</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B104" s="26">
-        <f>$D$43*(1+$B$72)^-A104*(1+$B$71)^A104</f>
+        <f t="shared" si="2"/>
         <v>36594207.37657769</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B105" s="26">
-        <f>$D$43*(1+$B$72)^-A105*(1+$B$71)^A105</f>
+        <f t="shared" si="2"/>
         <v>35921230.977505982</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B106" s="26">
-        <f>$D$43*(1+$B$72)^-A106*(1+$B$71)^A106</f>
+        <f t="shared" ref="B106:B134" si="4">$D$43*(1+$B$72)^-A106*(1+$B$71)^A106</f>
         <v>35260630.778553814</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B107" s="26">
-        <f>$D$43*(1+$B$72)^-A107*(1+$B$71)^A107</f>
+        <f t="shared" si="4"/>
         <v>34612179.178382367</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B108" s="26">
-        <f>$D$43*(1+$B$72)^-A108*(1+$B$71)^A108</f>
+        <f t="shared" si="4"/>
         <v>33975652.761296995</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B109" s="26">
-        <f>$D$43*(1+$B$72)^-A109*(1+$B$71)^A109</f>
+        <f t="shared" si="4"/>
         <v>33350832.220272169</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B110" s="26">
-        <f>$D$43*(1+$B$72)^-A110*(1+$B$71)^A110</f>
+        <f t="shared" si="4"/>
         <v>32737502.281392049</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="B111" s="26">
-        <f>$D$43*(1+$B$72)^-A111*(1+$B$71)^A111</f>
+        <f t="shared" si="4"/>
         <v>32135451.629680596</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="B112" s="26">
-        <f>$D$43*(1+$B$72)^-A112*(1+$B$71)^A112</f>
+        <f t="shared" si="4"/>
         <v>31544472.83629575</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="B113" s="26">
-        <f>$D$43*(1+$B$72)^-A113*(1+$B$71)^A113</f>
+        <f t="shared" si="4"/>
         <v>30964362.287062407</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="B114" s="26">
-        <f>$D$43*(1+$B$72)^-A114*(1+$B$71)^A114</f>
+        <f t="shared" si="4"/>
         <v>30394920.112319853</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="B115" s="26">
-        <f>$D$43*(1+$B$72)^-A115*(1+$B$71)^A115</f>
+        <f t="shared" si="4"/>
         <v>29835950.118059143</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116">
         <f>A115+1</f>
         <v>42</v>
       </c>
       <c r="B116" s="26">
-        <f>$D$43*(1+$B$72)^-A116*(1+$B$71)^A116</f>
+        <f t="shared" si="4"/>
         <v>29287259.718327034</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="B117" s="26">
-        <f>$D$43*(1+$B$72)^-A117*(1+$B$71)^A117</f>
+        <f t="shared" si="4"/>
         <v>28748659.868872918</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="B118" s="26">
-        <f>$D$43*(1+$B$72)^-A118*(1+$B$71)^A118</f>
+        <f t="shared" si="4"/>
         <v>28219965.002016105</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119">
         <f>A118+1</f>
         <v>45</v>
       </c>
       <c r="B119" s="26">
-        <f>$D$43*(1+$B$72)^-A119*(1+$B$71)^A119</f>
+        <f t="shared" si="4"/>
         <v>27700992.962710731</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="B120" s="26">
-        <f>$D$43*(1+$B$72)^-A120*(1+$B$71)^A120</f>
+        <f t="shared" si="4"/>
         <v>27191564.945786737</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="B121" s="26">
-        <f>$D$43*(1+$B$72)^-A121*(1+$B$71)^A121</f>
+        <f t="shared" si="4"/>
         <v>26691505.434344709</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="B122" s="26">
-        <f>$D$43*(1+$B$72)^-A122*(1+$B$71)^A122</f>
+        <f t="shared" si="4"/>
         <v>26200642.139283836</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="B123" s="26">
-        <f>$D$43*(1+$B$72)^-A123*(1+$B$71)^A123</f>
+        <f t="shared" si="4"/>
         <v>25718805.939941891</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="B124" s="26">
-        <f>$D$43*(1+$B$72)^-A124*(1+$B$71)^A124</f>
+        <f t="shared" si="4"/>
         <v>25245830.825826861</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="B125" s="26">
-        <f>$D$43*(1+$B$72)^-A125*(1+$B$71)^A125</f>
+        <f t="shared" si="4"/>
         <v>24781553.839420192</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="B126" s="26">
-        <f>$D$43*(1+$B$72)^-A126*(1+$B$71)^A126</f>
+        <f t="shared" si="4"/>
         <v>24325815.020031836</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="B127" s="26">
-        <f>$D$43*(1+$B$72)^-A127*(1+$B$71)^A127</f>
+        <f t="shared" si="4"/>
         <v>23878457.348687839</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="B128" s="26">
-        <f>$D$43*(1+$B$72)^-A128*(1+$B$71)^A128</f>
+        <f t="shared" si="4"/>
         <v>23439326.694031488</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="B129" s="26">
-        <f>$D$43*(1+$B$72)^-A129*(1+$B$71)^A129</f>
+        <f t="shared" si="4"/>
         <v>23008271.759219296</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="B130" s="26">
-        <f>$D$43*(1+$B$72)^-A130*(1+$B$71)^A130</f>
+        <f t="shared" si="4"/>
         <v>22585144.029793661</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="B131" s="26">
-        <f>$D$43*(1+$B$72)^-A131*(1+$B$71)^A131</f>
+        <f t="shared" si="4"/>
         <v>22169797.722514044</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132">
         <f>A131+1</f>
         <v>58</v>
       </c>
       <c r="B132" s="26">
-        <f>$D$43*(1+$B$72)^-A132*(1+$B$71)^A132</f>
+        <f t="shared" si="4"/>
         <v>21762089.735129274</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="B133" s="26">
-        <f>$D$43*(1+$B$72)^-A133*(1+$B$71)^A133</f>
+        <f t="shared" si="4"/>
         <v>21361879.59707348</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="B134" s="26">
-        <f>$D$43*(1+$B$72)^-A134*(1+$B$71)^A134</f>
+        <f t="shared" si="4"/>
         <v>20969029.421068776</v>
       </c>
     </row>
@@ -2963,29 +2947,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60C3FA1-C501-488F-99EF-B28CB9021ECA}">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A38" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="5" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="31.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1"/>
+    <col min="4" max="5" width="19.453125" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" customWidth="1"/>
+    <col min="9" max="9" width="15.6328125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.5" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" customWidth="1"/>
+    <col min="14" max="14" width="11.6328125" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>82</v>
       </c>
@@ -2996,25 +2980,25 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="G2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="G3" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="51">
+      <c r="H3" s="50">
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -3029,7 +3013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>102</v>
@@ -3045,7 +3029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -3061,7 +3045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="G8" t="s">
         <v>54</v>
@@ -3070,7 +3054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>88</v>
       </c>
@@ -3086,7 +3070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="G10" t="s">
         <v>57</v>
@@ -3098,7 +3082,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="G11" t="s">
         <v>58</v>
@@ -3107,7 +3091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>101</v>
       </c>
@@ -3118,7 +3102,6 @@
       <c r="D12" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="49"/>
       <c r="H12" s="13"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -3127,7 +3110,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -3157,7 +3140,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="36" t="s">
         <v>45</v>
       </c>
@@ -3184,7 +3167,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="36" t="s">
         <v>6</v>
       </c>
@@ -3206,7 +3189,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
         <v>5</v>
       </c>
@@ -3233,7 +3216,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B17" s="36" t="s">
         <v>49</v>
       </c>
@@ -3258,7 +3241,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="G18" t="s">
         <v>100</v>
@@ -3273,7 +3256,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="G19" t="s">
         <v>106</v>
       </c>
@@ -3287,14 +3270,14 @@
       <c r="M19" s="1"/>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="G20" s="1"/>
       <c r="I20" s="1"/>
       <c r="K20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H21" s="3" t="s">
         <v>73</v>
       </c>
@@ -3303,7 +3286,7 @@
       </c>
       <c r="K21" s="33"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H22" s="21"/>
       <c r="I22" s="21" t="s">
         <v>10</v>
@@ -3322,7 +3305,7 @@
       </c>
       <c r="R22" s="22"/>
     </row>
-    <row r="23" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="G23" t="s">
         <v>12</v>
       </c>
@@ -3360,7 +3343,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B24" s="48"/>
       <c r="C24" s="47" t="s">
         <v>98</v>
@@ -3412,7 +3395,7 @@
         <v>311.57375999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>0</v>
       </c>
@@ -3468,7 +3451,7 @@
       </c>
       <c r="R25" s="19"/>
     </row>
-    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B26" s="48" t="s">
         <v>2</v>
       </c>
@@ -3511,7 +3494,7 @@
       </c>
       <c r="R26" s="19"/>
     </row>
-    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B27" s="48" t="s">
         <v>10</v>
       </c>
@@ -3554,7 +3537,7 @@
       </c>
       <c r="R27" s="19"/>
     </row>
-    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B28" s="48" t="s">
         <v>8</v>
       </c>
@@ -3576,7 +3559,7 @@
       <c r="P28" s="3"/>
       <c r="R28" s="19"/>
     </row>
-    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B29" s="48" t="s">
         <v>87</v>
       </c>
@@ -3589,7 +3572,7 @@
         <v>308095.26507177029</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B30" s="36" t="s">
         <v>11</v>
       </c>
@@ -3602,11 +3585,11 @@
         <v>564144.1110047847</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>89</v>
       </c>
@@ -3622,10 +3605,10 @@
         <v>29335493.772248805</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="43" t="s">
         <v>15</v>
       </c>
@@ -3637,36 +3620,36 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="53" t="s">
+      <c r="C45" s="37" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>90</v>
       </c>
-      <c r="C46" s="52">
+      <c r="C46" s="51">
         <f>B34</f>
         <v>0.54231319391634991</v>
       </c>
@@ -3674,19 +3657,19 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>50</v>
       </c>
       <c r="C47">
-        <f t="dataTable" ref="C47:C48" dt2D="0" dtr="0" r1="H19" ca="1"/>
+        <f t="dataTable" ref="C47:C48" dt2D="0" dtr="0" r1="H19"/>
         <v>0.43291745247148294</v>
       </c>
       <c r="D47" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>185</v>
       </c>
@@ -3697,7 +3680,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>111</v>
       </c>
@@ -3708,17 +3691,17 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="50">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B51" s="49">
         <v>0.05</v>
       </c>
-      <c r="C51" s="52">
+      <c r="C51" s="51">
         <f>B34</f>
         <v>0.54231319391634991</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B52" s="50">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B52" s="49">
         <v>0.01</v>
       </c>
       <c r="C52">
@@ -3726,31 +3709,31 @@
         <v>2.7115659695817498</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="50">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B53" s="49">
         <v>0.03</v>
       </c>
       <c r="C53">
         <v>0.90385532319391648</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="50">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B54" s="49">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C54">
         <v>0.38736656708310707</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="50">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B55" s="49">
         <v>0.1</v>
       </c>
       <c r="C55">
         <v>0.27115659695817496</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -3758,8 +3741,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D58" s="52">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D58" s="51">
         <f>B34</f>
         <v>0.54231319391634991</v>
       </c>
@@ -3773,7 +3756,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -3787,7 +3770,7 @@
         <v>1.9789999999999999E-2</v>
       </c>
       <c r="E59">
-        <f t="dataTable" ref="E59:G61" dt2D="1" dtr="1" r1="H19" r2="Q24"/>
+        <f t="dataTable" ref="E59:G61" dt2D="1" dtr="1" r1="H19" r2="Q24" ca="1"/>
         <v>0.54231319391634991</v>
       </c>
       <c r="F59">
@@ -3797,7 +3780,7 @@
         <v>0.78845361216730037</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C60" s="8" t="s">
         <v>117</v>
       </c>
@@ -3814,8 +3797,8 @@
         <v>0.67187019011406846</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="52"/>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B61" s="51"/>
       <c r="C61" s="8" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
changed pop est, up tax op costs, discounted tax
</commit_message>
<xml_diff>
--- a/CBA (3).xlsx
+++ b/CBA (3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a630b34756993743/Desktop/ETHZ/Transport Planning Methods/TransportPlanning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanelmaheinonen/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{B60C97A6-90D9-F948-ACE4-80043545B60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F29F5F7-B2EB-4507-BDC2-5AFE9F4893D1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF90EC0-BD04-1344-9085-629596AE9AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="1" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tunnel" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -191,7 +194,7 @@
     <author>Heinonen  Sanelma</author>
   </authors>
   <commentList>
-    <comment ref="M23" authorId="0" shapeId="0" xr:uid="{FFC213B8-785A-9245-B331-3D07429FD761}">
+    <comment ref="M25" authorId="0" shapeId="0" xr:uid="{FFC213B8-785A-9245-B331-3D07429FD761}">
       <text>
         <r>
           <rPr>
@@ -235,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O23" authorId="0" shapeId="0" xr:uid="{482EA1DD-0C12-154A-9271-9F30C0517CFD}">
+    <comment ref="O25" authorId="0" shapeId="0" xr:uid="{482EA1DD-0C12-154A-9271-9F30C0517CFD}">
       <text>
         <r>
           <rPr>
@@ -268,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q23" authorId="0" shapeId="0" xr:uid="{7D0ECDC4-038D-9540-AF8A-68B4DAE10E75}">
+    <comment ref="Q25" authorId="0" shapeId="0" xr:uid="{7D0ECDC4-038D-9540-AF8A-68B4DAE10E75}">
       <text>
         <r>
           <rPr>
@@ -306,7 +309,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="138">
   <si>
     <t>Weekly benefits</t>
   </si>
@@ -624,9 +627,6 @@
     <t>Induced demand travel time savings (CHF)</t>
   </si>
   <si>
-    <t>Current adult population of Canton Zurich</t>
-  </si>
-  <si>
     <t>Cost of tax to drivers (counted as a negative benefit)</t>
   </si>
   <si>
@@ -745,6 +745,24 @@
   </si>
   <si>
     <t>Benefit-Cost Ratio</t>
+  </si>
+  <si>
+    <t>Current population of Canton Zurich</t>
+  </si>
+  <si>
+    <t>Annual Calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swiss Population Growth </t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>Lifecycle Costs (discounted, 60 yrs)</t>
+  </si>
+  <si>
+    <t>Lifecycle Benefits (discounted, 60 yrs)</t>
   </si>
 </sst>
 </file>
@@ -760,7 +778,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,6 +851,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -872,7 +899,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -935,13 +962,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1026,6 +1097,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1043,10 +1122,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1348,30 +1423,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083A40F-175A-4EEC-B4D7-09BE1D9F546C}">
   <dimension ref="A1:R134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView topLeftCell="A42" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" customWidth="1"/>
-    <col min="4" max="4" width="47.453125" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" customWidth="1"/>
-    <col min="6" max="6" width="18.36328125" customWidth="1"/>
-    <col min="7" max="7" width="29.81640625" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" customWidth="1"/>
-    <col min="10" max="11" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="47.5" customWidth="1"/>
+    <col min="5" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="11" width="17.5" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="11.81640625" customWidth="1"/>
-    <col min="16" max="16" width="12.81640625" customWidth="1"/>
-    <col min="17" max="17" width="11.36328125" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>43</v>
       </c>
@@ -1379,7 +1454,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1390,13 +1465,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C4" s="1"/>
       <c r="G4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1420,7 +1495,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1435,7 +1510,7 @@
         <v>65000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1450,7 +1525,7 @@
         <v>320000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1465,7 +1540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -1480,7 +1555,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +1570,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -1510,7 +1585,7 @@
         <v>4200000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
         <v>40</v>
       </c>
@@ -1518,7 +1593,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="G13" t="s">
@@ -1530,13 +1605,13 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
         <v>25</v>
       </c>
@@ -1554,7 +1629,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="C16" s="9" t="s">
         <v>28</v>
       </c>
@@ -1569,7 +1644,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1578,14 +1653,14 @@
         <v>71710187.283656985</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="G18" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
@@ -1604,7 +1679,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
@@ -1620,7 +1695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="G21" t="s">
@@ -1630,7 +1705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="28" t="s">
         <v>81</v>
       </c>
@@ -1647,7 +1722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
       <c r="D23" s="5"/>
       <c r="F23" s="6"/>
@@ -1661,7 +1736,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
       <c r="D24" s="5"/>
       <c r="F24" s="6"/>
@@ -1672,9 +1747,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="35" t="s">
         <v>47</v>
@@ -1691,7 +1766,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -1712,7 +1787,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="34" t="s">
         <v>45</v>
@@ -1731,7 +1806,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="34" t="s">
         <v>6</v>
@@ -1746,7 +1821,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="34" t="s">
         <v>5</v>
@@ -1765,7 +1840,7 @@
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="34" t="s">
         <v>49</v>
@@ -1780,13 +1855,13 @@
       </c>
       <c r="F30" s="6"/>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="H30" s="46">
-        <v>1240000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1520000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
@@ -1803,23 +1878,23 @@
       </c>
       <c r="F31" s="6"/>
       <c r="G31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H31" s="7">
         <v>1254</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C32" s="1"/>
       <c r="D32" s="5"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C33" s="1"/>
       <c r="D33" s="5"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>
       <c r="D34" s="3"/>
       <c r="F34" s="6"/>
@@ -1827,11 +1902,11 @@
         <v>73</v>
       </c>
       <c r="I34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K34" s="33"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C35" s="1"/>
       <c r="D35" s="5"/>
       <c r="F35" s="6"/>
@@ -1853,12 +1928,12 @@
       </c>
       <c r="R35" s="22"/>
     </row>
-    <row r="36" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="C36" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G36" t="s">
         <v>12</v>
@@ -1897,7 +1972,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>0</v>
       </c>
@@ -1910,7 +1985,7 @@
       </c>
       <c r="D37" s="26">
         <f>C37*($H$30/$H$31)</f>
-        <v>1199797.894736842</v>
+        <v>1470719.9999999998</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>3</v>
@@ -1955,7 +2030,7 @@
         <v>12.899999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="48" t="s">
         <v>8</v>
       </c>
@@ -1965,7 +2040,7 @@
       </c>
       <c r="D38" s="26">
         <f t="shared" ref="D38:D41" si="0">C38*($H$30/$H$31)</f>
-        <v>15572.382775119619</v>
+        <v>19088.727272727272</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>4</v>
@@ -2008,7 +2083,7 @@
       </c>
       <c r="R38" s="19"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="34" t="s">
         <v>63</v>
       </c>
@@ -2018,7 +2093,7 @@
       </c>
       <c r="D39" s="26">
         <f t="shared" si="0"/>
-        <v>12755.980861244017</v>
+        <v>15636.363636363632</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>6</v>
@@ -2050,7 +2125,7 @@
       </c>
       <c r="R39" s="19"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="D40" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2085,7 +2160,7 @@
       </c>
       <c r="R40" s="19"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="36" t="s">
         <v>49</v>
       </c>
@@ -2095,14 +2170,14 @@
       </c>
       <c r="D41" s="26">
         <f t="shared" si="0"/>
-        <v>1228126.2583732058</v>
+        <v>1505445.0909090906</v>
       </c>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>89</v>
       </c>
@@ -2112,48 +2187,48 @@
       </c>
       <c r="D43" s="2">
         <f>52*D41</f>
-        <v>63862565.4354067</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>78283144.727272704</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="27" t="s">
         <v>75</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="31">
         <f>SUM(B74:B134)</f>
-        <v>2353376160.1742077</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+        <v>2884783680.2135434</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B48" s="42">
         <f>D45/D22</f>
-        <v>1.1601565562363165</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1.4221273915154842</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B51" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>123</v>
-      </c>
-      <c r="B51" t="s">
-        <v>122</v>
-      </c>
       <c r="D51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" s="49">
         <v>1</v>
       </c>
@@ -2162,10 +2237,10 @@
       </c>
       <c r="D52" s="51">
         <f>B48</f>
-        <v>1.1601565562363165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1.4221273915154842</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53" s="49">
         <v>0.5</v>
       </c>
@@ -2173,11 +2248,11 @@
         <v>1014249390.5343409</v>
       </c>
       <c r="D53" s="51">
-        <f t="dataTable" ref="D53:D56" dt2D="0" dtr="0" r1="D22" ca="1"/>
-        <v>2.3203131124726331</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="dataTable" ref="D53:D56" dt2D="0" dtr="0" r1="D22"/>
+        <v>2.8442547830309683</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B54" s="49">
         <v>0.75</v>
       </c>
@@ -2185,10 +2260,10 @@
         <v>1521374085.8015113</v>
       </c>
       <c r="D54" s="51">
-        <v>1.5468754083150889</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1.8961698553539788</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B55" s="49">
         <v>1.5</v>
       </c>
@@ -2196,10 +2271,10 @@
         <v>3042748171.6030226</v>
       </c>
       <c r="D55" s="51">
-        <v>0.77343770415754443</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.94808492767698938</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B56" s="49">
         <v>2</v>
       </c>
@@ -2207,76 +2282,76 @@
         <v>4056997562.1373634</v>
       </c>
       <c r="D56" s="51">
-        <v>0.58007827811815826</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.71106369575774209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B58" s="53">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C58" s="51">
         <f>B48</f>
-        <v>1.1601565562363165</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1.4221273915154842</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B59" s="53">
         <v>0.05</v>
       </c>
       <c r="C59" s="51">
         <f t="dataTable" ref="C59:C61" dt2D="0" dtr="0" r1="H13" ca="1"/>
-        <v>0.71054629453694962</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.87099223201303466</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="45">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C60" s="51">
-        <v>0.52847290598642149</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.64780549766077467</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B61" s="53">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="C61" s="51">
-        <v>1.4766559831584645</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1.8100944309684392</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="23"/>
       <c r="C62" s="51"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" t="s">
         <v>131</v>
       </c>
-      <c r="C64" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B65">
         <f>H38</f>
@@ -2284,27 +2359,27 @@
       </c>
       <c r="C65" s="52">
         <f>B48</f>
-        <v>1.1601565562363165</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1.4221273915154842</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B66">
         <v>20.8</v>
       </c>
       <c r="C66" s="52">
-        <f t="dataTable" ref="C66" dt2D="0" dtr="0" r1="H38"/>
-        <v>1.6638881136021531</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+        <f t="dataTable" ref="C66" dt2D="0" dtr="0" r1="H38" ca="1"/>
+        <v>2.0396047844155416</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -2313,7 +2388,7 @@
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -2322,7 +2397,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2330,611 +2405,611 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>0</v>
       </c>
       <c r="B74" s="26">
-        <f t="shared" ref="B74:B105" si="2">$D$43*(1+$B$72)^-A74*(1+$B$71)^A74</f>
-        <v>63862565.4354067</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+        <f>$D$43*(1+$B$72)^-A74*(1+$B$71)^A74</f>
+        <v>78283144.727272704</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1</v>
       </c>
       <c r="B75" s="26">
-        <f t="shared" si="2"/>
-        <v>62688117.280814111</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+        <f t="shared" ref="B74:B105" si="2">$D$43*(1+$B$72)^-A75*(1+$B$71)^A75</f>
+        <v>76843498.602288246</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2</v>
       </c>
       <c r="B76" s="26">
         <f t="shared" si="2"/>
-        <v>61535267.514235236</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+        <v>75430327.920675427</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <f>A76+1</f>
         <v>3</v>
       </c>
       <c r="B77" s="26">
         <f t="shared" si="2"/>
-        <v>60403618.936046623</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+        <v>74043145.792573258</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" ref="A78:A134" si="3">A77+1</f>
         <v>4</v>
       </c>
       <c r="B78" s="26">
         <f t="shared" si="2"/>
-        <v>59292781.651222758</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+        <v>72681474.28214401</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B79" s="26">
         <f t="shared" si="2"/>
-        <v>58202372.935002707</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+        <v>71344844.242906526</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B80" s="26">
         <f t="shared" si="2"/>
-        <v>57132017.101027302</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+        <v>70032795.156097963</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B81" s="26">
         <f t="shared" si="2"/>
-        <v>56081345.371901102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+        <v>68744874.972007781</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B82" s="26">
         <f t="shared" si="2"/>
-        <v>55049995.752134927</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+        <v>67480639.954229891</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B83" s="26">
         <f t="shared" si="2"/>
-        <v>54037612.903424948</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+        <v>66239654.526778951</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B84" s="26">
         <f t="shared" si="2"/>
-        <v>53043848.02222538</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+        <v>65021491.124018192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B85" s="26">
         <f t="shared" si="2"/>
-        <v>52068358.719572745</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+        <v>63825730.043347217</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B86" s="26">
         <f t="shared" si="2"/>
-        <v>51110808.903120138</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+        <v>62651959.30059886</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B87" s="26">
         <f t="shared" si="2"/>
-        <v>50170868.661340795</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+        <v>61499774.488095157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B88" s="26">
         <f t="shared" si="2"/>
-        <v>49248214.149861522</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+        <v>60368778.635314107</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B89" s="26">
         <f t="shared" si="2"/>
-        <v>48342527.479886018</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+        <v>59258582.072118327</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90">
         <f>A89+1</f>
         <v>16</v>
       </c>
       <c r="B90" s="26">
         <f t="shared" si="2"/>
-        <v>47453496.608670563</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+        <v>58168802.294499375</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B91" s="26">
         <f t="shared" si="2"/>
-        <v>46580815.232013553</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+        <v>57099063.832790792</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B92" s="26">
         <f t="shared" si="2"/>
-        <v>45724182.678722374</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+        <v>56048998.122304827</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B93" s="26">
         <f t="shared" si="2"/>
-        <v>44883303.807020999</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+        <v>55018243.376348302</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B94" s="26">
         <f t="shared" si="2"/>
-        <v>44057888.902862623</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+        <v>54006444.461573519</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B95" s="26">
         <f t="shared" si="2"/>
-        <v>43247653.580112427</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+        <v>53013252.775621668</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B96" s="26">
         <f t="shared" si="2"/>
-        <v>42452318.682565972</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52038326.127016336</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B97" s="26">
         <f t="shared" si="2"/>
-        <v>41671610.187769525</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+        <v>51081328.617265843</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B98" s="26">
         <f t="shared" si="2"/>
-        <v>40905259.112609081</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+        <v>50141930.525133699</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B99" s="26">
         <f t="shared" si="2"/>
-        <v>40153001.42063573</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+        <v>49219808.193037339</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B100" s="26">
         <f t="shared" si="2"/>
-        <v>39414577.93109528</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+        <v>48314643.915536135</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B101" s="26">
         <f t="shared" si="2"/>
-        <v>38689734.229630738</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47426125.829869926</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B102" s="26">
         <f t="shared" si="2"/>
-        <v>37978220.5806273</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+        <v>46553947.808510877</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
         <f>A102+1</f>
         <v>29</v>
       </c>
       <c r="B103" s="26">
         <f t="shared" si="2"/>
-        <v>37279791.841168925</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+        <v>45697809.353690922</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B104" s="26">
         <f t="shared" si="2"/>
-        <v>36594207.37657769</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+        <v>44857415.493869409</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B105" s="26">
         <f t="shared" si="2"/>
-        <v>35921230.977505982</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+        <v>44032476.682104088</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B106" s="26">
         <f t="shared" ref="B106:B134" si="4">$D$43*(1+$B$72)^-A106*(1+$B$71)^A106</f>
-        <v>35260630.778553814</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+        <v>43222708.69629176</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B107" s="26">
         <f t="shared" si="4"/>
-        <v>34612179.178382367</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+        <v>42427832.54124289</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B108" s="26">
         <f t="shared" si="4"/>
-        <v>33975652.761296995</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41647574.3525576</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B109" s="26">
         <f t="shared" si="4"/>
-        <v>33350832.220272169</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+        <v>40881665.302269101</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B110" s="26">
         <f t="shared" si="4"/>
-        <v>32737502.281392049</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+        <v>40129841.506222501</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="B111" s="26">
         <f t="shared" si="4"/>
-        <v>32135451.629680596</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+        <v>39391843.933156848</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="B112" s="26">
         <f t="shared" si="4"/>
-        <v>31544472.83629575</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+        <v>38667418.315459296</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="B113" s="26">
         <f t="shared" si="4"/>
-        <v>30964362.287062407</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+        <v>37956315.061560355</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="B114" s="26">
         <f t="shared" si="4"/>
-        <v>30394920.112319853</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+        <v>37258289.169940449</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="B115" s="26">
         <f t="shared" si="4"/>
-        <v>29835950.118059143</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+        <v>36573100.144717649</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
         <f>A115+1</f>
         <v>42</v>
       </c>
       <c r="B116" s="26">
         <f t="shared" si="4"/>
-        <v>29287259.718327034</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+        <v>35900511.912787966</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="B117" s="26">
         <f t="shared" si="4"/>
-        <v>28748659.868872918</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+        <v>35240292.742489375</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="B118" s="26">
         <f t="shared" si="4"/>
-        <v>28219965.002016105</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+        <v>34592215.16376166</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
         <f>A118+1</f>
         <v>45</v>
       </c>
       <c r="B119" s="26">
         <f t="shared" si="4"/>
-        <v>27700992.962710731</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+        <v>33956055.889774427</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="B120" s="26">
         <f t="shared" si="4"/>
-        <v>27191564.945786737</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+        <v>33331595.739996634</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="B121" s="26">
         <f t="shared" si="4"/>
-        <v>26691505.434344709</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+        <v>32718619.564680599</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="B122" s="26">
         <f t="shared" si="4"/>
-        <v>26200642.139283836</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+        <v>32116916.170735013</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="B123" s="26">
         <f t="shared" si="4"/>
-        <v>25718805.939941891</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+        <v>31526278.248961017</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="B124" s="26">
         <f t="shared" si="4"/>
-        <v>25245830.825826861</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+        <v>30946502.302626465</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="B125" s="26">
         <f t="shared" si="4"/>
-        <v>24781553.839420192</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+        <v>30377388.577353776</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="B126" s="26">
         <f t="shared" si="4"/>
-        <v>24325815.020031836</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29818740.992297079</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="B127" s="26">
         <f t="shared" si="4"/>
-        <v>23878457.348687839</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29270367.072585084</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="B128" s="26">
         <f t="shared" si="4"/>
-        <v>23439326.694031488</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28732077.883006334</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="B129" s="26">
         <f t="shared" si="4"/>
-        <v>23008271.759219296</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28203687.962913968</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="B130" s="26">
         <f t="shared" si="4"/>
-        <v>22585144.029793661</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27685015.262327705</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="B131" s="26">
         <f t="shared" si="4"/>
-        <v>22169797.722514044</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27175881.079210754</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
         <f>A131+1</f>
         <v>58</v>
       </c>
       <c r="B132" s="26">
         <f t="shared" si="4"/>
-        <v>21762089.735129274</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+        <v>26676109.997900393</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="B133" s="26">
         <f t="shared" si="4"/>
-        <v>21361879.59707348</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+        <v>26185529.82867071</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="B134" s="26">
         <f t="shared" si="4"/>
-        <v>20969029.421068776</v>
+        <v>25703971.548406877</v>
       </c>
     </row>
   </sheetData>
@@ -2945,31 +3020,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60C3FA1-C501-488F-99EF-B28CB9021ECA}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="5" width="19.453125" customWidth="1"/>
-    <col min="7" max="7" width="31.81640625" customWidth="1"/>
-    <col min="8" max="8" width="14.6328125" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="5" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" customWidth="1"/>
-    <col min="13" max="13" width="10.6328125" customWidth="1"/>
-    <col min="14" max="14" width="11.6328125" customWidth="1"/>
-    <col min="16" max="16" width="12.453125" customWidth="1"/>
-    <col min="18" max="18" width="12.81640625" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.5" customWidth="1"/>
+    <col min="18" max="18" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>82</v>
       </c>
@@ -2977,188 +3052,148 @@
         <v>83</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="G2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="H2" s="13">
+        <v>6.1500000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="G3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="50">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+      <c r="H3" s="24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="G4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1520000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="26">
-        <f>10*D13*H17/H18</f>
-        <v>20805103.668261562</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="B7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="26">
+        <f>10*D15*H4/H19</f>
+        <v>25503030.303030305</v>
+      </c>
+      <c r="G7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="50">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="2">
+        <f xml:space="preserve"> H7*C7</f>
+        <v>2550303.0303030307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5">
+        <f>C8</f>
+        <v>2550303.0303030307</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="2">
-        <f xml:space="preserve"> H3*C5</f>
-        <v>1040255.1834130781</v>
-      </c>
-      <c r="G6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5">
-        <f>C6</f>
-        <v>1040255.1834130781</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="40">
-        <f>C7*52</f>
-        <v>54093269.537480056</v>
-      </c>
-      <c r="G9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="40">
+        <f>C9*52</f>
+        <v>132615757.57575759</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H14" s="7">
         <v>17</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-      <c r="G11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="7">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="7">
-        <v>3416</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2104</v>
-      </c>
-      <c r="E13">
-        <f>D13-C13</f>
-        <v>-1312</v>
-      </c>
-      <c r="G13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="13">
-        <v>25</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="7">
-        <v>2742</v>
-      </c>
-      <c r="D14" s="7">
-        <v>3089</v>
-      </c>
-      <c r="E14">
-        <f t="shared" ref="E14:E16" si="0">D14-C14</f>
-        <v>347</v>
-      </c>
-      <c r="G14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="13">
-        <v>20</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -3167,21 +3202,29 @@
       <c r="M14" s="1"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="B15" s="36" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" s="7">
-        <v>3119</v>
+        <v>3416</v>
       </c>
       <c r="D15" s="7">
-        <v>3514</v>
+        <v>2104</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>395</v>
-      </c>
-      <c r="H15" s="1"/>
+        <f>D15-C15</f>
+        <v>-1312</v>
+      </c>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="7">
+        <v>27</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="4"/>
@@ -3189,26 +3232,21 @@
       <c r="M15" s="1"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="36" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7">
-        <v>235</v>
+        <v>2742</v>
       </c>
       <c r="D16" s="7">
-        <v>265</v>
+        <v>3089</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="13">
-        <v>6.1500000000000001E-3</v>
-      </c>
+        <f t="shared" ref="E16:E18" si="0">D16-C16</f>
+        <v>347</v>
+      </c>
+      <c r="H16" s="13"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="4"/>
@@ -3216,23 +3254,25 @@
       <c r="M16" s="1"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17">
-        <f>SUM(C13:C16)</f>
-        <v>9512</v>
-      </c>
-      <c r="D17">
-        <f>SUM(D13:D16)</f>
-        <v>8972</v>
+        <v>6</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3119</v>
+      </c>
+      <c r="D17" s="7">
+        <v>3514</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>395</v>
       </c>
       <c r="G17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" s="7">
-        <v>1240000</v>
+        <v>59</v>
+      </c>
+      <c r="H17" s="13">
+        <v>25</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -3241,13 +3281,25 @@
       <c r="M17" s="1"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B18" s="1"/>
+    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7">
+        <v>235</v>
+      </c>
+      <c r="D18" s="7">
+        <v>265</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="G18" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" s="1">
-        <v>1254</v>
+        <v>60</v>
+      </c>
+      <c r="H18" s="13">
+        <v>20</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -3256,12 +3308,23 @@
       <c r="M18" s="1"/>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C15:C18)</f>
+        <v>9512</v>
+      </c>
+      <c r="D19">
+        <f>SUM(D15:D18)</f>
+        <v>8972</v>
+      </c>
       <c r="G19" t="s">
-        <v>106</v>
-      </c>
-      <c r="H19" s="13">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1254</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -3270,549 +3333,1474 @@
       <c r="M19" s="1"/>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="G20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="13">
+        <v>90</v>
+      </c>
       <c r="I20" s="1"/>
-      <c r="K20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="H21" s="3" t="s">
+      <c r="J20" s="1"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="K22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K21" s="33"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="H22" s="21"/>
-      <c r="I22" s="21" t="s">
+      <c r="I23" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23" s="33"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H24" s="21"/>
+      <c r="I24" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17" t="s">
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="22" t="s">
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="R22" s="22"/>
-    </row>
-    <row r="23" spans="1:18" ht="87" x14ac:dyDescent="0.35">
-      <c r="G23" t="s">
+      <c r="R24" s="22"/>
+    </row>
+    <row r="25" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P23" s="4" t="s">
+      <c r="P25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B24" s="48"/>
-      <c r="C24" s="47" t="s">
+    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="48"/>
+      <c r="C26" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H26" s="7">
         <v>23.3</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I26" s="15">
         <v>0</v>
       </c>
-      <c r="J24" s="38">
+      <c r="J26" s="38">
         <v>0</v>
       </c>
-      <c r="K24" s="39">
-        <f>I24+J24</f>
+      <c r="K26" s="39">
+        <f>I26+J26</f>
         <v>0</v>
       </c>
-      <c r="L24">
-        <f>C13*H6-D13*H6</f>
+      <c r="L26">
+        <f>C15*H10-D15*H10</f>
         <v>15744</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M26" s="7">
         <v>192</v>
       </c>
-      <c r="N24">
-        <f>M24/1000000</f>
+      <c r="N26">
+        <f>M26/1000000</f>
         <v>1.92E-4</v>
       </c>
-      <c r="O24" s="7">
-        <f>$H$19</f>
+      <c r="O26" s="7">
+        <f>$H$20</f>
         <v>90</v>
       </c>
-      <c r="P24" s="3">
-        <f>L24*N24*O24</f>
+      <c r="P26" s="3">
+        <f>L26*N26*O26</f>
         <v>272.05632000000003</v>
       </c>
-      <c r="Q24" s="7">
+      <c r="Q26" s="7">
         <f>0.012*0.59+0.031*0.41</f>
         <v>1.9789999999999999E-2</v>
       </c>
-      <c r="R24">
-        <f>L24*Q24</f>
+      <c r="R26">
+        <f>L26*Q26</f>
         <v>311.57375999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B27" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="26">
-        <f>-10*D13</f>
+      <c r="C27" s="26">
+        <f>-10*D15</f>
         <v>-21040</v>
       </c>
-      <c r="D25" s="26">
-        <f>C25*$H$17/$H$18</f>
-        <v>-20805103.668261562</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="D27" s="26">
+        <f>C27*$H$4/$H$19</f>
+        <v>-25503030.303030305</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H27" s="7">
         <v>14.4</v>
       </c>
-      <c r="I25">
+      <c r="I27">
         <v>0</v>
       </c>
-      <c r="J25" s="38">
-        <f>0.5*(D14-C14)*(H11-H11)*H25</f>
+      <c r="J27" s="38">
+        <f>0.5*(D16-C16)*(H15-H15)*H27</f>
         <v>0</v>
       </c>
-      <c r="K25" s="39">
-        <f>I25+J25</f>
+      <c r="K27" s="39">
+        <f>I27+J27</f>
         <v>0</v>
       </c>
-      <c r="L25">
-        <f>C14*H7-D14*H7</f>
+      <c r="L27">
+        <f>C16*H11-D16*H11</f>
         <v>-4164</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M27" s="7">
         <v>35</v>
       </c>
-      <c r="N25">
-        <f t="shared" ref="N25:N27" si="1">M25/1000000</f>
+      <c r="N27">
+        <f t="shared" ref="N27:N29" si="1">M27/1000000</f>
         <v>3.4999999999999997E-5</v>
       </c>
-      <c r="O25" s="7">
-        <f t="shared" ref="O25:O27" si="2">$H$19</f>
+      <c r="O27" s="7">
+        <f>$H$20</f>
         <v>90</v>
       </c>
-      <c r="P25" s="3">
-        <f>L25*N25*O25</f>
+      <c r="P27" s="3">
+        <f>L27*N27*O27</f>
         <v>-13.116599999999998</v>
       </c>
-      <c r="Q25">
+      <c r="Q27">
         <v>0</v>
       </c>
-      <c r="R25" s="19"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B26" s="48" t="s">
+      <c r="R27" s="19"/>
+    </row>
+    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="26">
-        <f>10*D13</f>
+      <c r="C28" s="26">
+        <f>10*D15</f>
         <v>21040</v>
       </c>
-      <c r="D26" s="26">
-        <f>C26*$H$17/$H$18</f>
-        <v>20805103.668261562</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="D28" s="26">
+        <f>C28*$H$4/$H$19</f>
+        <v>25503030.303030305</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="18"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26">
-        <f>D15*H8-C15*H8</f>
+      <c r="H28" s="18"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28">
+        <f>D17*H12-C17*H12</f>
         <v>790</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M28" s="7">
         <v>0</v>
       </c>
-      <c r="N26">
+      <c r="N28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O26" s="7">
-        <f t="shared" si="2"/>
+      <c r="O28" s="7">
+        <f>$H$20</f>
         <v>90</v>
       </c>
-      <c r="P26" s="3">
-        <f>L26*N26*O26</f>
+      <c r="P28" s="3">
+        <f>L28*N28*O28</f>
         <v>0</v>
       </c>
-      <c r="Q26">
+      <c r="Q28">
         <v>0</v>
       </c>
-      <c r="R26" s="19"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B27" s="48" t="s">
+      <c r="R28" s="19"/>
+    </row>
+    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="26">
-        <f>SUM(K24:K27)</f>
+      <c r="C29" s="26">
+        <f>SUM(K26:K29)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="26">
-        <f>C27*$H$17/$H$18</f>
+      <c r="D29" s="26">
+        <f>C29*$H$4/$H$19</f>
         <v>0</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27">
-        <f>D16*H9-C16*H9</f>
+      <c r="H29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29">
+        <f>D18*H13-C18*H13</f>
         <v>150</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M29" s="7">
         <v>0</v>
       </c>
-      <c r="N27">
+      <c r="N29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O27" s="7">
-        <f t="shared" si="2"/>
+      <c r="O29" s="7">
+        <f>$H$20</f>
         <v>90</v>
       </c>
-      <c r="P27" s="3">
-        <f>L27*M27*O27</f>
+      <c r="P29" s="3">
+        <f>L29*M29*O29</f>
         <v>0</v>
       </c>
-      <c r="Q27">
+      <c r="Q29">
         <v>0</v>
       </c>
-      <c r="R27" s="19"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B28" s="48" t="s">
+      <c r="R29" s="19"/>
+    </row>
+    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="26">
-        <f>SUM(P24:P27)</f>
+      <c r="C30" s="26">
+        <f>SUM(P26:P29)</f>
         <v>258.93972000000002</v>
       </c>
-      <c r="D28" s="26">
-        <f>C28*$H$17/$H$18</f>
-        <v>256048.84593301435</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="M28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="3"/>
-      <c r="R28" s="19"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B29" s="48" t="s">
+      <c r="D30" s="26">
+        <f>C30*$H$4/$H$19</f>
+        <v>313866.32727272733</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="M30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="3"/>
+      <c r="R30" s="19"/>
+    </row>
+    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="26">
-        <f>SUM(R24:R27)</f>
+      <c r="C31" s="26">
+        <f>SUM(R26:R29)</f>
         <v>311.57375999999999</v>
       </c>
-      <c r="D29" s="26">
-        <f>C29*$H$17/$H$18</f>
-        <v>308095.26507177029</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B30" s="36" t="s">
+      <c r="D31" s="26">
+        <f>C31*$H$4/$H$19</f>
+        <v>377665.16363636364</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="40">
-        <f>SUM(C25:C29)</f>
+      <c r="C32" s="40">
+        <f>SUM(C27:C31)</f>
         <v>570.51348000000007</v>
       </c>
-      <c r="D30" s="40">
-        <f>SUM(D25:D29)</f>
-        <v>564144.1110047847</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="D32" s="40">
+        <f>SUM(D27:D31)</f>
+        <v>691531.49090909096</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="40">
-        <f>C30*52</f>
+      <c r="C34" s="40">
+        <f>C32*52</f>
         <v>29666.700960000002</v>
       </c>
-      <c r="D32" s="40">
-        <f>D30*52</f>
-        <v>29335493.772248805</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="43" t="s">
+      <c r="D34" s="40">
+        <f>D32*52</f>
+        <v>35959637.527272731</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="57">
+        <f>SUM(C71:C131)</f>
+        <v>4886975025.4223013</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="59">
+        <f>SUM(B71:B131)</f>
+        <v>1325135517.3131018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="44">
-        <f>D32/C9</f>
+      <c r="B40" s="44">
+        <f>B37/B36</f>
+        <v>0.27115659695817496</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>90</v>
+      </c>
+      <c r="C48" s="51">
+        <f>B40</f>
+        <v>0.27115659695817496</v>
+      </c>
+      <c r="D48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <f t="dataTable" ref="C49:C50" dt2D="0" dtr="0" r1="H20"/>
+        <v>0.21645872623574136</v>
+      </c>
+      <c r="D49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>185</v>
+      </c>
+      <c r="C50">
+        <v>0.40106403992395434</v>
+      </c>
+      <c r="D50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B53" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="C53" s="51">
+        <f>B40</f>
+        <v>0.27115659695817496</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B54" s="49">
+        <v>0.05</v>
+      </c>
+      <c r="C54">
+        <f t="dataTable" ref="C54:C57" dt2D="0" dtr="0" r1="H7" ca="1"/>
         <v>0.54231319391634991</v>
       </c>
-      <c r="C34" s="8" t="s">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="49">
+        <v>0.15</v>
+      </c>
+      <c r="C55">
+        <v>0.18077106463878342</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B56" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C56">
+        <v>0.10846263878327005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B57" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="C57">
+        <v>5.4231319391635023E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B45" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="37" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B46">
+      <c r="E59" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D60" s="51">
+        <f>B40</f>
+        <v>0.27115659695817496</v>
+      </c>
+      <c r="E60" s="7">
         <v>90</v>
       </c>
-      <c r="C46" s="51">
-        <f>B34</f>
-        <v>0.54231319391634991</v>
-      </c>
-      <c r="D46" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B47">
-        <v>50</v>
-      </c>
-      <c r="C47">
-        <f t="dataTable" ref="C47:C48" dt2D="0" dtr="0" r1="H19"/>
-        <v>0.43291745247148294</v>
-      </c>
-      <c r="D47" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B48">
-        <v>185</v>
-      </c>
-      <c r="C48">
-        <v>0.80212807984790879</v>
-      </c>
-      <c r="D48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="C50" s="37" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B51" s="49">
-        <v>0.05</v>
-      </c>
-      <c r="C51" s="51">
-        <f>B34</f>
-        <v>0.54231319391634991</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B52" s="49">
-        <v>0.01</v>
-      </c>
-      <c r="C52">
-        <f t="dataTable" ref="C52:C55" dt2D="0" dtr="0" r1="H3" ca="1"/>
-        <v>2.7115659695817498</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B53" s="49">
-        <v>0.03</v>
-      </c>
-      <c r="C53">
-        <v>0.90385532319391648</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B54" s="49">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C54">
-        <v>0.38736656708310707</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B55" s="49">
-        <v>0.1</v>
-      </c>
-      <c r="C55">
-        <v>0.27115659695817496</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="F60" s="7">
+        <v>0</v>
+      </c>
+      <c r="G60" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D58" s="51">
-        <f>B34</f>
-        <v>0.54231319391634991</v>
-      </c>
-      <c r="E58" s="7">
-        <v>90</v>
-      </c>
-      <c r="F58" s="7">
-        <v>0</v>
-      </c>
-      <c r="G58" s="7">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>120</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D59" s="7">
-        <v>1.9789999999999999E-2</v>
-      </c>
-      <c r="E59">
-        <f t="dataTable" ref="E59:G61" dt2D="1" dtr="1" r1="H19" r2="Q24" ca="1"/>
-        <v>0.54231319391634991</v>
-      </c>
-      <c r="F59">
-        <v>0.29617277566539923</v>
-      </c>
-      <c r="G59">
-        <v>0.78845361216730037</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C60" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D60" s="7">
-        <v>1.2E-2</v>
-      </c>
-      <c r="E60">
-        <v>0.42572977186311795</v>
-      </c>
-      <c r="F60">
-        <v>0.17958935361216735</v>
-      </c>
-      <c r="G60">
-        <v>0.67187019011406846</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B61" s="51"/>
       <c r="C61" s="8" t="s">
         <v>118</v>
       </c>
       <c r="D61" s="7">
+        <v>1.9789999999999999E-2</v>
+      </c>
+      <c r="E61">
+        <f t="dataTable" ref="E61:G63" dt2D="1" dtr="1" r1="H20" r2="Q26" ca="1"/>
+        <v>0.27115659695817496</v>
+      </c>
+      <c r="F61">
+        <v>0.14808638783269956</v>
+      </c>
+      <c r="G61">
+        <v>0.39422680608365013</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C62" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="7">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E62">
+        <v>0.21286488593155897</v>
+      </c>
+      <c r="F62">
+        <v>8.9794676806083579E-2</v>
+      </c>
+      <c r="G62">
+        <v>0.33593509505703412</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B63" s="51"/>
+      <c r="C63" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" s="7">
         <v>3.1E-2</v>
       </c>
-      <c r="E61">
-        <v>0.71007958174904962</v>
-      </c>
-      <c r="F61">
-        <v>0.46393916349809894</v>
-      </c>
-      <c r="G61">
-        <v>0.95622000000000018</v>
+      <c r="E63">
+        <v>0.35503979087452447</v>
+      </c>
+      <c r="F63">
+        <v>0.23196958174904936</v>
+      </c>
+      <c r="G63">
+        <v>0.47810999999999987</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="55">
+        <f>H2</f>
+        <v>6.1500000000000001E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" s="55">
+        <f>H3</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="B71" s="26">
+        <f>$D$34*(1+$B$68)^-A71*(1+$B$67)^A71</f>
+        <v>35959637.527272731</v>
+      </c>
+      <c r="C71" s="26">
+        <f>$C$11*(1+$B$68)^-A71*(1+$B$67)^A71</f>
+        <v>132615757.57575759</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <f>A71+1</f>
+        <v>1</v>
+      </c>
+      <c r="B72" s="26">
+        <f t="shared" ref="B72:B130" si="2">$D$34*(1+$B$68)^-A72*(1+$B$67)^A72</f>
+        <v>35298331.022502892</v>
+      </c>
+      <c r="C72" s="26">
+        <f t="shared" ref="C72:C131" si="3">$C$11*(1+$B$68)^-A72*(1+$B$67)^A72</f>
+        <v>130176921.44863272</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <f t="shared" ref="A73:A131" si="4">A72+1</f>
+        <v>2</v>
+      </c>
+      <c r="B73" s="26">
+        <f t="shared" si="2"/>
+        <v>34649186.105650038</v>
+      </c>
+      <c r="C73" s="26">
+        <f t="shared" si="3"/>
+        <v>127782936.11272371</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="B74" s="26">
+        <f t="shared" si="2"/>
+        <v>34011979.12214613</v>
+      </c>
+      <c r="C74" s="26">
+        <f t="shared" si="3"/>
+        <v>125432976.75104095</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="B75" s="26">
+        <f t="shared" si="2"/>
+        <v>33386490.530485213</v>
+      </c>
+      <c r="C75" s="26">
+        <f t="shared" si="3"/>
+        <v>123126233.71518038</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="B76" s="26">
+        <f t="shared" si="2"/>
+        <v>32772504.826583117</v>
+      </c>
+      <c r="C76" s="26">
+        <f t="shared" si="3"/>
+        <v>120861912.2463695</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="B77" s="26">
+        <f t="shared" si="2"/>
+        <v>32169810.469528399</v>
+      </c>
+      <c r="C77" s="26">
+        <f t="shared" si="3"/>
+        <v>118639232.2016436</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="B78" s="26">
+        <f t="shared" si="2"/>
+        <v>31578199.808698539</v>
+      </c>
+      <c r="C78" s="26">
+        <f t="shared" si="3"/>
+        <v>116457427.78505729</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="B79" s="26">
+        <f t="shared" si="2"/>
+        <v>30997469.012216624</v>
+      </c>
+      <c r="C79" s="26">
+        <f t="shared" si="3"/>
+        <v>114315747.28383943</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B80" s="26">
+        <f t="shared" si="2"/>
+        <v>30427417.996723674</v>
+      </c>
+      <c r="C80" s="26">
+        <f t="shared" si="3"/>
+        <v>112213452.80940007</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B81" s="26">
+        <f t="shared" si="2"/>
+        <v>29867850.358442467</v>
+      </c>
+      <c r="C81" s="26">
+        <f t="shared" si="3"/>
+        <v>110149820.04310037</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="B82" s="26">
+        <f t="shared" si="2"/>
+        <v>29318573.305509154</v>
+      </c>
+      <c r="C82" s="26">
+        <f t="shared" si="3"/>
+        <v>108124137.98669799</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="B83" s="26">
+        <f t="shared" si="2"/>
+        <v>28779397.591549315</v>
+      </c>
+      <c r="C83" s="26">
+        <f t="shared" si="3"/>
+        <v>106135708.71738169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="B84" s="26">
+        <f t="shared" si="2"/>
+        <v>28250137.450475451</v>
+      </c>
+      <c r="C84" s="26">
+        <f t="shared" si="3"/>
+        <v>104183847.14731079</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="B85" s="26">
+        <f t="shared" si="2"/>
+        <v>27730610.532483794</v>
+      </c>
+      <c r="C85" s="26">
+        <f t="shared" si="3"/>
+        <v>102267880.78757736</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="B86" s="26">
+        <f t="shared" si="2"/>
+        <v>27220637.841227867</v>
+      </c>
+      <c r="C86" s="26">
+        <f t="shared" si="3"/>
+        <v>100387149.51650824</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="B87" s="26">
+        <f t="shared" si="2"/>
+        <v>26720043.672147729</v>
+      </c>
+      <c r="C87" s="26">
+        <f t="shared" si="3"/>
+        <v>98541005.352229044</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="B88" s="26">
+        <f t="shared" si="2"/>
+        <v>26228655.551933117</v>
+      </c>
+      <c r="C88" s="26">
+        <f t="shared" si="3"/>
+        <v>96728812.229410037</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="B89" s="26">
+        <f t="shared" si="2"/>
+        <v>25746304.179099999</v>
+      </c>
+      <c r="C89" s="26">
+        <f t="shared" si="3"/>
+        <v>94949945.780117944</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="B90" s="26">
+        <f t="shared" si="2"/>
+        <v>25272823.365659971</v>
+      </c>
+      <c r="C90" s="26">
+        <f t="shared" si="3"/>
+        <v>93203793.118698224</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="B91" s="26">
+        <f t="shared" si="2"/>
+        <v>24808049.979862232</v>
+      </c>
+      <c r="C91" s="26">
+        <f t="shared" si="3"/>
+        <v>91489752.630612925</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="B92" s="26">
+        <f t="shared" si="2"/>
+        <v>24351823.889988668</v>
+      </c>
+      <c r="C92" s="26">
+        <f t="shared" si="3"/>
+        <v>89807233.765162155</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="B93" s="26">
+        <f t="shared" si="2"/>
+        <v>23903987.909182541</v>
+      </c>
+      <c r="C93" s="26">
+        <f t="shared" si="3"/>
+        <v>88155656.832017466</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="B94" s="26">
+        <f t="shared" si="2"/>
+        <v>23464387.741291724</v>
+      </c>
+      <c r="C94" s="26">
+        <f t="shared" si="3"/>
+        <v>86534452.801496983</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="B95" s="26">
+        <f t="shared" si="2"/>
+        <v>23032871.92770797</v>
+      </c>
+      <c r="C95" s="26">
+        <f t="shared" si="3"/>
+        <v>84943063.108513355</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="B96" s="26">
+        <f t="shared" si="2"/>
+        <v>22609291.795183785</v>
+      </c>
+      <c r="C96" s="26">
+        <f t="shared" si="3"/>
+        <v>83380939.460127518</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="B97" s="26">
+        <f t="shared" si="2"/>
+        <v>22193501.404608946</v>
+      </c>
+      <c r="C97" s="26">
+        <f t="shared" si="3"/>
+        <v>81847543.646641314</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="B98" s="26">
+        <f t="shared" si="2"/>
+        <v>21785357.500729062</v>
+      </c>
+      <c r="C98" s="26">
+        <f t="shared" si="3"/>
+        <v>80342347.356164038</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="B99" s="26">
+        <f t="shared" si="2"/>
+        <v>21384719.462788835</v>
+      </c>
+      <c r="C99" s="26">
+        <f t="shared" si="3"/>
+        <v>78864831.992589742</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="B100" s="26">
+        <f>$D$34*(1+$B$68)^-A100*(1+$B$67)^A100</f>
+        <v>20991449.256082904</v>
+      </c>
+      <c r="C100" s="26">
+        <f t="shared" si="3"/>
+        <v>77414488.496921107</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="B101" s="26">
+        <f t="shared" si="2"/>
+        <v>20605411.384397879</v>
+      </c>
+      <c r="C101" s="26">
+        <f t="shared" si="3"/>
+        <v>75990817.171880215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="B102" s="26">
+        <f t="shared" si="2"/>
+        <v>20226472.843328703</v>
+      </c>
+      <c r="C102" s="26">
+        <f t="shared" si="3"/>
+        <v>74593327.509743661</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="B103" s="26">
+        <f t="shared" si="2"/>
+        <v>19854503.074453834</v>
+      </c>
+      <c r="C103" s="26">
+        <f t="shared" si="3"/>
+        <v>73221538.023344979</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="B104" s="26">
+        <f t="shared" si="2"/>
+        <v>19489373.92035291</v>
+      </c>
+      <c r="C104" s="26">
+        <f t="shared" si="3"/>
+        <v>71874976.080183983</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="B105" s="26">
+        <f t="shared" si="2"/>
+        <v>19130959.580451787</v>
+      </c>
+      <c r="C105" s="26">
+        <f t="shared" si="3"/>
+        <v>70553177.739587426</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="B106" s="26">
+        <f t="shared" si="2"/>
+        <v>18779136.567679577</v>
+      </c>
+      <c r="C106" s="26">
+        <f t="shared" si="3"/>
+        <v>69255687.59286429</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="B107" s="26">
+        <f t="shared" si="2"/>
+        <v>18433783.665922739</v>
+      </c>
+      <c r="C107" s="26">
+        <f t="shared" si="3"/>
+        <v>67982058.6064004</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="B108" s="26">
+        <f t="shared" si="2"/>
+        <v>18094781.888261624</v>
+      </c>
+      <c r="C108" s="26">
+        <f t="shared" si="3"/>
+        <v>66731851.967638798</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="B109" s="26">
+        <f t="shared" si="2"/>
+        <v>17762014.435975064</v>
+      </c>
+      <c r="C109" s="26">
+        <f t="shared" si="3"/>
+        <v>65504636.933892503</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <f>A109+1</f>
+        <v>39</v>
+      </c>
+      <c r="B110" s="26">
+        <f t="shared" si="2"/>
+        <v>17435366.658298839</v>
+      </c>
+      <c r="C110" s="26">
+        <f t="shared" si="3"/>
+        <v>64299990.68393749</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="B111" s="26">
+        <f t="shared" si="2"/>
+        <v>17114726.012924273</v>
+      </c>
+      <c r="C111" s="26">
+        <f t="shared" si="3"/>
+        <v>63117498.172335342</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="B112" s="26">
+        <f t="shared" si="2"/>
+        <v>16799982.027223181</v>
+      </c>
+      <c r="C112" s="26">
+        <f t="shared" si="3"/>
+        <v>61956751.986434348</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="B113" s="26">
+        <f t="shared" si="2"/>
+        <v>16491026.260185955</v>
+      </c>
+      <c r="C113" s="26">
+        <f t="shared" si="3"/>
+        <v>60817352.206000909</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="B114" s="26">
+        <f t="shared" si="2"/>
+        <v>16187752.265059607</v>
+      </c>
+      <c r="C114" s="26">
+        <f t="shared" si="3"/>
+        <v>59698906.265431993</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="B115" s="26">
+        <f t="shared" si="2"/>
+        <v>15890055.552672913</v>
+      </c>
+      <c r="C115" s="26">
+        <f t="shared" si="3"/>
+        <v>58601028.818501905</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="B116" s="26">
+        <f t="shared" si="2"/>
+        <v>15597833.555435946</v>
+      </c>
+      <c r="C116" s="26">
+        <f t="shared" si="3"/>
+        <v>57523341.605595782</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="B117" s="26">
+        <f t="shared" si="2"/>
+        <v>15310985.592001837</v>
+      </c>
+      <c r="C117" s="26">
+        <f t="shared" si="3"/>
+        <v>56465473.323385566</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="B118" s="26">
+        <f t="shared" si="2"/>
+        <v>15029412.832578193</v>
+      </c>
+      <c r="C118" s="26">
+        <f t="shared" si="3"/>
+        <v>55427059.49690184</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="B119" s="26">
+        <f t="shared" si="2"/>
+        <v>14753018.264876636</v>
+      </c>
+      <c r="C119" s="26">
+        <f t="shared" si="3"/>
+        <v>54407742.353958823</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="B120" s="26">
+        <f t="shared" si="2"/>
+        <v>14481706.660688419</v>
+      </c>
+      <c r="C120" s="26">
+        <f t="shared" si="3"/>
+        <v>53407170.701888472</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="B121" s="26">
+        <f t="shared" si="2"/>
+        <v>14215384.543074783</v>
+      </c>
+      <c r="C121" s="26">
+        <f t="shared" si="3"/>
+        <v>52424999.806541555</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <f>A121+1</f>
+        <v>51</v>
+      </c>
+      <c r="B122" s="26">
+        <f t="shared" si="2"/>
+        <v>13953960.154160677</v>
+      </c>
+      <c r="C122" s="26">
+        <f t="shared" si="3"/>
+        <v>51460891.273513928</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <f t="shared" si="4"/>
+        <v>52</v>
+      </c>
+      <c r="B123" s="26">
+        <f>$D$34*(1+$B$68)^-A123*(1+$B$67)^A123</f>
+        <v>13697343.423520749</v>
+      </c>
+      <c r="C123" s="26">
+        <f t="shared" si="3"/>
+        <v>50514512.931557126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="B124" s="26">
+        <f t="shared" si="2"/>
+        <v>13445445.937146734</v>
+      </c>
+      <c r="C124" s="26">
+        <f t="shared" si="3"/>
+        <v>49585538.718132883</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="B125" s="26">
+        <f t="shared" si="2"/>
+        <v>13198180.906985551</v>
+      </c>
+      <c r="C125" s="26">
+        <f t="shared" si="3"/>
+        <v>48673648.567072593</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="B126" s="26">
+        <f t="shared" si="2"/>
+        <v>12955463.141037574</v>
+      </c>
+      <c r="C126" s="26">
+        <f t="shared" si="3"/>
+        <v>47778528.298302531</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="B127" s="26">
+        <f t="shared" si="2"/>
+        <v>12717209.014004838</v>
+      </c>
+      <c r="C127" s="26">
+        <f t="shared" si="3"/>
+        <v>46899869.509597175</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="B128" s="26">
+        <f t="shared" si="2"/>
+        <v>12483336.438478993</v>
+      </c>
+      <c r="C128" s="26">
+        <f t="shared" si="3"/>
+        <v>46037369.470323123</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <f>A128+1</f>
+        <v>58</v>
+      </c>
+      <c r="B129" s="26">
+        <f t="shared" si="2"/>
+        <v>12253764.836659163</v>
+      </c>
+      <c r="C129" s="26">
+        <f t="shared" si="3"/>
+        <v>45190731.017137192</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="B130" s="26">
+        <f t="shared" si="2"/>
+        <v>12028415.112589866</v>
+      </c>
+      <c r="C130" s="26">
+        <f t="shared" si="3"/>
+        <v>44359662.451602511</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="B131" s="26">
+        <f>$D$34*(1+$B$68)^-A131*(1+$B$67)^A131</f>
+        <v>11807209.624909563</v>
+      </c>
+      <c r="C131" s="26">
+        <f t="shared" si="3"/>
+        <v>43543877.439687699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected tunnel signal costs and VAT
</commit_message>
<xml_diff>
--- a/CBA (3).xlsx
+++ b/CBA (3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanelmaheinonen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a630b34756993743/Desktop/ETHZ/Transport Planning Methods/TransportPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF90EC0-BD04-1344-9085-629596AE9AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{4BF90EC0-BD04-1344-9085-629596AE9AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7F0B680-43A2-4E8F-91AB-DBDBEC5D1674}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="1" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tunnel" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -309,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
   <si>
     <t>Weekly benefits</t>
   </si>
@@ -413,15 +410,6 @@
     <t>Costs:</t>
   </si>
   <si>
-    <t>EW Switch per unit</t>
-  </si>
-  <si>
-    <t># of EW Switch</t>
-  </si>
-  <si>
-    <t>Tunnel construction per track km</t>
-  </si>
-  <si>
     <t># tracks built</t>
   </si>
   <si>
@@ -429,9 +417,6 @@
   </si>
   <si>
     <t xml:space="preserve">Interlocking Station </t>
-  </si>
-  <si>
-    <t>Signals</t>
   </si>
   <si>
     <t>VAT rate (tax)</t>
@@ -763,6 +748,24 @@
   </si>
   <si>
     <t>Lifecycle Benefits (discounted, 60 yrs)</t>
+  </si>
+  <si>
+    <t>Tunnel construction (per meter)</t>
+  </si>
+  <si>
+    <t>EW Switch (per unit)</t>
+  </si>
+  <si>
+    <t># of EW Switches</t>
+  </si>
+  <si>
+    <t>Slab track (per meter)</t>
+  </si>
+  <si>
+    <t>Catenary (per meter)</t>
+  </si>
+  <si>
+    <t>Signal (per unit)</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1015,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1098,7 +1101,6 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1423,38 +1425,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083A40F-175A-4EEC-B4D7-09BE1D9F546C}">
   <dimension ref="A1:R134"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="47.5" customWidth="1"/>
-    <col min="5" max="5" width="5.5" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="11" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" customWidth="1"/>
+    <col min="4" max="4" width="47.453125" customWidth="1"/>
+    <col min="5" max="5" width="5.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.36328125" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" customWidth="1"/>
+    <col min="10" max="11" width="17.453125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" customWidth="1"/>
+    <col min="17" max="17" width="11.36328125" customWidth="1"/>
+    <col min="18" max="18" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1465,13 +1467,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C4" s="1"/>
       <c r="G4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1486,16 +1488,16 @@
         <v>1040000000</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H5" s="7">
         <v>2</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1504,13 +1506,13 @@
         <v>1280000</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="H6" s="7">
         <v>65000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1519,13 +1521,13 @@
         <v>35200000</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="H7" s="7">
         <v>320000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1534,13 +1536,13 @@
         <v>7520000</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="H8" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -1549,51 +1551,51 @@
         <v>4200000</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="H9" s="7">
         <v>2200</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="10">
-        <f>(D3*H12*H5)/2</f>
-        <v>640000000</v>
+        <f>(D3*H12*H5)/2000</f>
+        <v>640000</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="H10" s="7">
         <v>470</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="5">
         <f>SUM(D5:D10)</f>
-        <v>1728200000</v>
+        <v>1088840000</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H11" s="7">
         <v>4200000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G12" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="H12" s="7">
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="G13" t="s">
@@ -1605,13 +1607,13 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B15" s="11" t="s">
         <v>25</v>
       </c>
@@ -1623,13 +1625,13 @@
         <v>52672669.125554681</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H15" s="7">
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C16" s="9" t="s">
         <v>28</v>
       </c>
@@ -1638,13 +1640,13 @@
         <v>19037518.158102311</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H16" s="7">
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1653,122 +1655,122 @@
         <v>71710187.283656985</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="G18" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="2">
         <f>H16*(D11+D17)</f>
-        <v>89995509.36418286</v>
+        <v>58027509.36418286</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H19" s="7">
         <v>15</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="2">
-        <f>(D17+D11)*H15</f>
-        <v>138593084.4208416</v>
+        <f>(D17+D11+D19)*H15</f>
+        <v>93830482.641883686</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H20" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H21" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="32">
         <f>D11+D17+D19+D20</f>
-        <v>2028498781.0686817</v>
+        <v>1312408179.2897236</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H22" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
       <c r="D23" s="5"/>
       <c r="F23" s="6"/>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H23" s="7">
         <v>18</v>
       </c>
       <c r="I23" s="33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="5"/>
       <c r="F24" s="6"/>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H24" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H25">
         <f>H24*(1-0.4)</f>
         <v>19.8</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>3</v>
@@ -1781,16 +1783,16 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H26" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="34" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C27" s="13">
         <v>322</v>
@@ -1800,13 +1802,13 @@
       </c>
       <c r="F27" s="6"/>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H27" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="34" t="s">
         <v>6</v>
@@ -1821,7 +1823,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="34" t="s">
         <v>5</v>
@@ -1834,16 +1836,16 @@
       </c>
       <c r="F29" s="6"/>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H29" s="24">
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="34" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1">
         <f>SUM(C26:C29)</f>
@@ -1855,18 +1857,18 @@
       </c>
       <c r="F30" s="6"/>
       <c r="G30" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H30" s="46">
         <v>1520000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C31" s="16">
         <f>C30*52</f>
@@ -1878,35 +1880,35 @@
       </c>
       <c r="F31" s="6"/>
       <c r="G31" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H31" s="7">
         <v>1254</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="5"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="5"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
       <c r="D34" s="3"/>
       <c r="F34" s="6"/>
       <c r="H34" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K34" s="33"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C35" s="1"/>
       <c r="D35" s="5"/>
       <c r="F35" s="6"/>
@@ -1918,22 +1920,22 @@
       <c r="K35" s="21"/>
       <c r="L35" s="17"/>
       <c r="M35" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N35" s="17"/>
       <c r="O35" s="17"/>
       <c r="P35" s="17"/>
       <c r="Q35" s="22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R35" s="22"/>
     </row>
-    <row r="36" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C36" s="35" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G36" t="s">
         <v>12</v>
@@ -1942,37 +1944,37 @@
         <v>7</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>0</v>
       </c>
@@ -2030,7 +2032,7 @@
         <v>12.899999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="48" t="s">
         <v>8</v>
       </c>
@@ -2083,9 +2085,9 @@
       </c>
       <c r="R38" s="19"/>
     </row>
-    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B39" s="34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C39" s="2">
         <f>SUM(R37:R40)</f>
@@ -2125,7 +2127,7 @@
       </c>
       <c r="R39" s="19"/>
     </row>
-    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D40" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2160,9 +2162,9 @@
       </c>
       <c r="R40" s="19"/>
     </row>
-    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B41" s="36" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C41" s="2">
         <f>SUM(C37:C39)</f>
@@ -2174,12 +2176,12 @@
       </c>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C43" s="2">
         <f>52*C41</f>
@@ -2190,12 +2192,12 @@
         <v>78283144.727272704</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="31">
@@ -2203,32 +2205,32 @@
         <v>2884783680.2135434</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B48" s="42">
         <f>D45/D22</f>
-        <v>1.4221273915154842</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.1980841979930288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D51" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B52" s="49">
         <v>1</v>
       </c>
@@ -2237,10 +2239,10 @@
       </c>
       <c r="D52" s="51">
         <f>B48</f>
-        <v>1.4221273915154842</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.1980841979930288</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B53" s="49">
         <v>0.5</v>
       </c>
@@ -2248,11 +2250,11 @@
         <v>1014249390.5343409</v>
       </c>
       <c r="D53" s="51">
-        <f t="dataTable" ref="D53:D56" dt2D="0" dtr="0" r1="D22"/>
+        <f t="dataTable" ref="D53:D56" dt2D="0" dtr="0" r1="D22" ca="1"/>
         <v>2.8442547830309683</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B54" s="49">
         <v>0.75</v>
       </c>
@@ -2263,7 +2265,7 @@
         <v>1.8961698553539788</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B55" s="49">
         <v>1.5</v>
       </c>
@@ -2274,7 +2276,7 @@
         <v>0.94808492767698938</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B56" s="49">
         <v>2</v>
       </c>
@@ -2285,73 +2287,73 @@
         <v>0.71106369575774209</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="8" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="B58" s="53">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C58" s="51">
         <f>B48</f>
-        <v>1.4221273915154842</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.1980841979930288</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B59" s="53">
         <v>0.05</v>
       </c>
       <c r="C59" s="51">
-        <f t="dataTable" ref="C59:C61" dt2D="0" dtr="0" r1="H13" ca="1"/>
-        <v>0.87099223201303466</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="dataTable" ref="C59:C61" dt2D="0" dtr="0" r1="H13"/>
+        <v>1.359705633074098</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B60" s="45">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C60" s="51">
-        <v>0.64780549766077467</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.0156621236600862</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B61" s="53">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="C61" s="51">
-        <v>1.8100944309684392</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.7796056761386327</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
       <c r="B62" s="23"/>
       <c r="C62" s="51"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B65">
         <f>H38</f>
@@ -2359,53 +2361,53 @@
       </c>
       <c r="C65" s="52">
         <f>B48</f>
-        <v>1.4221273915154842</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2.1980841979930288</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B66">
         <v>20.8</v>
       </c>
       <c r="C66" s="52">
         <f t="dataTable" ref="C66" dt2D="0" dtr="0" r1="H38" ca="1"/>
-        <v>2.0396047844155416</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3.1524764050829881</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B71" s="23">
         <f>H29</f>
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B72" s="45">
         <f>H13</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>0</v>
       </c>
@@ -2414,16 +2416,16 @@
         <v>78283144.727272704</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
       <c r="B75" s="26">
-        <f t="shared" ref="B74:B105" si="2">$D$43*(1+$B$72)^-A75*(1+$B$71)^A75</f>
+        <f t="shared" ref="B75:B105" si="2">$D$43*(1+$B$72)^-A75*(1+$B$71)^A75</f>
         <v>76843498.602288246</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2</v>
       </c>
@@ -2432,7 +2434,7 @@
         <v>75430327.920675427</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
         <f>A76+1</f>
         <v>3</v>
@@ -2442,7 +2444,7 @@
         <v>74043145.792573258</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" ref="A78:A134" si="3">A77+1</f>
         <v>4</v>
@@ -2452,7 +2454,7 @@
         <v>72681474.28214401</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -2462,7 +2464,7 @@
         <v>71344844.242906526</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -2472,7 +2474,7 @@
         <v>70032795.156097963</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -2482,7 +2484,7 @@
         <v>68744874.972007781</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -2492,7 +2494,7 @@
         <v>67480639.954229891</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -2502,7 +2504,7 @@
         <v>66239654.526778951</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -2512,7 +2514,7 @@
         <v>65021491.124018192</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -2522,7 +2524,7 @@
         <v>63825730.043347217</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -2532,7 +2534,7 @@
         <v>62651959.30059886</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -2542,7 +2544,7 @@
         <v>61499774.488095157</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -2552,7 +2554,7 @@
         <v>60368778.635314107</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -2562,7 +2564,7 @@
         <v>59258582.072118327</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90">
         <f>A89+1</f>
         <v>16</v>
@@ -2572,7 +2574,7 @@
         <v>58168802.294499375</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -2582,7 +2584,7 @@
         <v>57099063.832790792</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -2592,7 +2594,7 @@
         <v>56048998.122304827</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -2602,7 +2604,7 @@
         <v>55018243.376348302</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -2612,7 +2614,7 @@
         <v>54006444.461573519</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -2622,7 +2624,7 @@
         <v>53013252.775621668</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -2632,7 +2634,7 @@
         <v>52038326.127016336</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -2642,7 +2644,7 @@
         <v>51081328.617265843</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -2652,7 +2654,7 @@
         <v>50141930.525133699</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -2662,7 +2664,7 @@
         <v>49219808.193037339</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -2672,7 +2674,7 @@
         <v>48314643.915536135</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -2682,7 +2684,7 @@
         <v>47426125.829869926</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -2692,7 +2694,7 @@
         <v>46553947.808510877</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103">
         <f>A102+1</f>
         <v>29</v>
@@ -2702,7 +2704,7 @@
         <v>45697809.353690922</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -2712,7 +2714,7 @@
         <v>44857415.493869409</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -2722,7 +2724,7 @@
         <v>44032476.682104088</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -2732,7 +2734,7 @@
         <v>43222708.69629176</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -2742,7 +2744,7 @@
         <v>42427832.54124289</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -2752,7 +2754,7 @@
         <v>41647574.3525576</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -2762,7 +2764,7 @@
         <v>40881665.302269101</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -2772,7 +2774,7 @@
         <v>40129841.506222501</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -2782,7 +2784,7 @@
         <v>39391843.933156848</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>38</v>
@@ -2792,7 +2794,7 @@
         <v>38667418.315459296</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113">
         <f t="shared" si="3"/>
         <v>39</v>
@@ -2802,7 +2804,7 @@
         <v>37956315.061560355</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114">
         <f t="shared" si="3"/>
         <v>40</v>
@@ -2812,7 +2814,7 @@
         <v>37258289.169940449</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115">
         <f t="shared" si="3"/>
         <v>41</v>
@@ -2822,7 +2824,7 @@
         <v>36573100.144717649</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116">
         <f>A115+1</f>
         <v>42</v>
@@ -2832,7 +2834,7 @@
         <v>35900511.912787966</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117">
         <f t="shared" si="3"/>
         <v>43</v>
@@ -2842,7 +2844,7 @@
         <v>35240292.742489375</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118">
         <f t="shared" si="3"/>
         <v>44</v>
@@ -2852,7 +2854,7 @@
         <v>34592215.16376166</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119">
         <f>A118+1</f>
         <v>45</v>
@@ -2862,7 +2864,7 @@
         <v>33956055.889774427</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120">
         <f t="shared" si="3"/>
         <v>46</v>
@@ -2872,7 +2874,7 @@
         <v>33331595.739996634</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -2882,7 +2884,7 @@
         <v>32718619.564680599</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -2892,7 +2894,7 @@
         <v>32116916.170735013</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -2902,7 +2904,7 @@
         <v>31526278.248961017</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -2912,7 +2914,7 @@
         <v>30946502.302626465</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125">
         <f t="shared" si="3"/>
         <v>51</v>
@@ -2922,7 +2924,7 @@
         <v>30377388.577353776</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126">
         <f t="shared" si="3"/>
         <v>52</v>
@@ -2932,7 +2934,7 @@
         <v>29818740.992297079</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127">
         <f t="shared" si="3"/>
         <v>53</v>
@@ -2942,7 +2944,7 @@
         <v>29270367.072585084</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128">
         <f t="shared" si="3"/>
         <v>54</v>
@@ -2952,7 +2954,7 @@
         <v>28732077.883006334</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>55</v>
@@ -2962,7 +2964,7 @@
         <v>28203687.962913968</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>56</v>
@@ -2972,7 +2974,7 @@
         <v>27685015.262327705</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>57</v>
@@ -2982,7 +2984,7 @@
         <v>27175881.079210754</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132">
         <f>A131+1</f>
         <v>58</v>
@@ -2992,7 +2994,7 @@
         <v>26676109.997900393</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>59</v>
@@ -3002,7 +3004,7 @@
         <v>26185529.82867071</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -3022,104 +3024,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60C3FA1-C501-488F-99EF-B28CB9021ECA}">
   <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="112" workbookViewId="0">
+    <sheetView zoomScale="112" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="5" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="31.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1"/>
+    <col min="4" max="5" width="19.453125" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" customWidth="1"/>
+    <col min="9" max="9" width="15.6328125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.5" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" customWidth="1"/>
+    <col min="14" max="14" width="11.6328125" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H2" s="13">
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="G3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H3" s="24">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="G4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H4" s="7">
         <v>1520000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="G6" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C7" s="26">
         <f>10*D15*H4/H19</f>
         <v>25503030.303030305</v>
       </c>
       <c r="G7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H7" s="50">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C8" s="2">
         <f xml:space="preserve"> H7*C7</f>
         <v>2550303.0303030307</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -3129,21 +3131,21 @@
         <v>2550303.0303030307</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H10" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="40">
@@ -3151,46 +3153,46 @@
         <v>132615757.57575759</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H11" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H12" s="7">
         <v>2</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H13" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="47" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D14" s="47" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H14" s="7">
         <v>17</v>
@@ -3202,9 +3204,9 @@
       <c r="M14" s="1"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>3</v>
@@ -3220,7 +3222,7 @@
         <v>-1312</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H15" s="7">
         <v>27</v>
@@ -3232,9 +3234,9 @@
       <c r="M15" s="1"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" s="7">
         <v>2742</v>
@@ -3254,7 +3256,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B17" s="36" t="s">
         <v>6</v>
       </c>
@@ -3269,7 +3271,7 @@
         <v>395</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H17" s="13">
         <v>25</v>
@@ -3281,7 +3283,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B18" s="36" t="s">
         <v>5</v>
       </c>
@@ -3296,7 +3298,7 @@
         <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H18" s="13">
         <v>20</v>
@@ -3308,9 +3310,9 @@
       <c r="M18" s="1"/>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B19" s="36" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <f>SUM(C15:C18)</f>
@@ -3321,7 +3323,7 @@
         <v>8972</v>
       </c>
       <c r="G19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H19" s="1">
         <v>1254</v>
@@ -3333,10 +3335,10 @@
       <c r="M19" s="1"/>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="G20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H20" s="13">
         <v>90</v>
@@ -3348,7 +3350,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="4"/>
@@ -3356,23 +3358,23 @@
       <c r="M21" s="1"/>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="G22" s="1"/>
       <c r="I22" s="1"/>
       <c r="K22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H23" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K23" s="33"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H24" s="21"/>
       <c r="I24" s="21" t="s">
         <v>10</v>
@@ -3381,17 +3383,17 @@
       <c r="K24" s="21"/>
       <c r="L24" s="17"/>
       <c r="M24" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R24" s="22"/>
     </row>
-    <row r="25" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="G25" t="s">
         <v>12</v>
       </c>
@@ -3399,43 +3401,43 @@
         <v>7</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B26" s="48"/>
       <c r="C26" s="47" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D26" s="47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>3</v>
@@ -3481,7 +3483,7 @@
         <v>311.57375999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>0</v>
       </c>
@@ -3537,7 +3539,7 @@
       </c>
       <c r="R27" s="19"/>
     </row>
-    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B28" s="48" t="s">
         <v>2</v>
       </c>
@@ -3580,7 +3582,7 @@
       </c>
       <c r="R28" s="19"/>
     </row>
-    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B29" s="48" t="s">
         <v>10</v>
       </c>
@@ -3623,7 +3625,7 @@
       </c>
       <c r="R29" s="19"/>
     </row>
-    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B30" s="48" t="s">
         <v>8</v>
       </c>
@@ -3645,9 +3647,9 @@
       <c r="P30" s="3"/>
       <c r="R30" s="19"/>
     </row>
-    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B31" s="48" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C31" s="26">
         <f>SUM(R26:R29)</f>
@@ -3658,7 +3660,7 @@
         <v>377665.16363636364</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B32" s="36" t="s">
         <v>11</v>
       </c>
@@ -3671,13 +3673,13 @@
         <v>691531.49090909096</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>11</v>
@@ -3691,34 +3693,34 @@
         <v>35959637.527272731</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="56" t="s">
-        <v>136</v>
-      </c>
-      <c r="B36" s="57">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="56">
         <f>SUM(C71:C131)</f>
         <v>4886975025.4223013</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="B37" s="59">
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="58">
         <f>SUM(B71:B131)</f>
         <v>1325135517.3131018</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="43" t="s">
         <v>15</v>
       </c>
@@ -3727,26 +3729,26 @@
         <v>0.27115659695817496</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>90</v>
       </c>
@@ -3755,10 +3757,10 @@
         <v>0.27115659695817496</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B49">
         <v>50</v>
       </c>
@@ -3767,10 +3769,10 @@
         <v>0.21645872623574136</v>
       </c>
       <c r="D49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B50">
         <v>185</v>
       </c>
@@ -3778,21 +3780,21 @@
         <v>0.40106403992395434</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C52" s="37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B53" s="49">
         <v>0.1</v>
       </c>
@@ -3801,7 +3803,7 @@
         <v>0.27115659695817496</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B54" s="49">
         <v>0.05</v>
       </c>
@@ -3810,7 +3812,7 @@
         <v>0.54231319391634991</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B55" s="49">
         <v>0.15</v>
       </c>
@@ -3818,7 +3820,7 @@
         <v>0.18077106463878342</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B56" s="49">
         <v>0.25</v>
       </c>
@@ -3826,7 +3828,7 @@
         <v>0.10846263878327005</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B57" s="49">
         <v>0.5</v>
       </c>
@@ -3834,15 +3836,15 @@
         <v>5.4231319391635023E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D60" s="51">
         <f>B40</f>
         <v>0.27115659695817496</v>
@@ -3857,15 +3859,15 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="D61" s="7">
         <v>1.9789999999999999E-2</v>
@@ -3881,9 +3883,9 @@
         <v>0.39422680608365013</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C62" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D62" s="7">
         <v>1.2E-2</v>
@@ -3898,10 +3900,10 @@
         <v>0.33593509505703412</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B63" s="51"/>
       <c r="C63" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D63" s="7">
         <v>3.1E-2</v>
@@ -3916,41 +3918,41 @@
         <v>0.47810999999999987</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="54" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>134</v>
-      </c>
-      <c r="B67" s="55">
+        <v>130</v>
+      </c>
+      <c r="B67" s="23">
         <f>H2</f>
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>123</v>
-      </c>
-      <c r="B68" s="55">
+        <v>119</v>
+      </c>
+      <c r="B68" s="23">
         <f>H3</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="47" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B70" s="47" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C70" s="47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>0</v>
       </c>
@@ -3963,7 +3965,7 @@
         <v>132615757.57575759</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
         <f>A71+1</f>
         <v>1</v>
@@ -3977,7 +3979,7 @@
         <v>130176921.44863272</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" ref="A73:A131" si="4">A72+1</f>
         <v>2</v>
@@ -3991,7 +3993,7 @@
         <v>127782936.11272371</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="4"/>
         <v>3</v>
@@ -4005,7 +4007,7 @@
         <v>125432976.75104095</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -4019,7 +4021,7 @@
         <v>123126233.71518038</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -4033,7 +4035,7 @@
         <v>120861912.2463695</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -4047,7 +4049,7 @@
         <v>118639232.2016436</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -4061,7 +4063,7 @@
         <v>116457427.78505729</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="4"/>
         <v>8</v>
@@ -4075,7 +4077,7 @@
         <v>114315747.28383943</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -4089,7 +4091,7 @@
         <v>112213452.80940007</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -4103,7 +4105,7 @@
         <v>110149820.04310037</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -4117,7 +4119,7 @@
         <v>108124137.98669799</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4131,7 +4133,7 @@
         <v>106135708.71738169</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -4145,7 +4147,7 @@
         <v>104183847.14731079</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -4159,7 +4161,7 @@
         <v>102267880.78757736</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -4173,7 +4175,7 @@
         <v>100387149.51650824</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -4187,7 +4189,7 @@
         <v>98541005.352229044</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -4201,7 +4203,7 @@
         <v>96728812.229410037</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -4215,7 +4217,7 @@
         <v>94949945.780117944</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
         <f t="shared" si="4"/>
         <v>19</v>
@@ -4229,7 +4231,7 @@
         <v>93203793.118698224</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -4243,7 +4245,7 @@
         <v>91489752.630612925</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="4"/>
         <v>21</v>
@@ -4257,7 +4259,7 @@
         <v>89807233.765162155</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="4"/>
         <v>22</v>
@@ -4271,7 +4273,7 @@
         <v>88155656.832017466</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="4"/>
         <v>23</v>
@@ -4285,7 +4287,7 @@
         <v>86534452.801496983</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -4299,7 +4301,7 @@
         <v>84943063.108513355</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="4"/>
         <v>25</v>
@@ -4313,7 +4315,7 @@
         <v>83380939.460127518</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="4"/>
         <v>26</v>
@@ -4327,7 +4329,7 @@
         <v>81847543.646641314</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="4"/>
         <v>27</v>
@@ -4341,7 +4343,7 @@
         <v>80342347.356164038</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="4"/>
         <v>28</v>
@@ -4355,7 +4357,7 @@
         <v>78864831.992589742</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" si="4"/>
         <v>29</v>
@@ -4369,7 +4371,7 @@
         <v>77414488.496921107</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="4"/>
         <v>30</v>
@@ -4383,7 +4385,7 @@
         <v>75990817.171880215</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="4"/>
         <v>31</v>
@@ -4397,7 +4399,7 @@
         <v>74593327.509743661</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103">
         <f t="shared" si="4"/>
         <v>32</v>
@@ -4411,7 +4413,7 @@
         <v>73221538.023344979</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="4"/>
         <v>33</v>
@@ -4425,7 +4427,7 @@
         <v>71874976.080183983</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
         <f t="shared" si="4"/>
         <v>34</v>
@@ -4439,7 +4441,7 @@
         <v>70553177.739587426</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="4"/>
         <v>35</v>
@@ -4453,7 +4455,7 @@
         <v>69255687.59286429</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="4"/>
         <v>36</v>
@@ -4467,7 +4469,7 @@
         <v>67982058.6064004</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="4"/>
         <v>37</v>
@@ -4481,7 +4483,7 @@
         <v>66731851.967638798</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="4"/>
         <v>38</v>
@@ -4495,7 +4497,7 @@
         <v>65504636.933892503</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
         <f>A109+1</f>
         <v>39</v>
@@ -4509,7 +4511,7 @@
         <v>64299990.68393749</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="4"/>
         <v>40</v>
@@ -4523,7 +4525,7 @@
         <v>63117498.172335342</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="4"/>
         <v>41</v>
@@ -4537,7 +4539,7 @@
         <v>61956751.986434348</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113">
         <f t="shared" si="4"/>
         <v>42</v>
@@ -4551,7 +4553,7 @@
         <v>60817352.206000909</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114">
         <f t="shared" si="4"/>
         <v>43</v>
@@ -4565,7 +4567,7 @@
         <v>59698906.265431993</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
         <f t="shared" si="4"/>
         <v>44</v>
@@ -4579,7 +4581,7 @@
         <v>58601028.818501905</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116">
         <f t="shared" si="4"/>
         <v>45</v>
@@ -4593,7 +4595,7 @@
         <v>57523341.605595782</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117">
         <f t="shared" si="4"/>
         <v>46</v>
@@ -4607,7 +4609,7 @@
         <v>56465473.323385566</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118">
         <f t="shared" si="4"/>
         <v>47</v>
@@ -4621,7 +4623,7 @@
         <v>55427059.49690184</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119">
         <f t="shared" si="4"/>
         <v>48</v>
@@ -4635,7 +4637,7 @@
         <v>54407742.353958823</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120">
         <f t="shared" si="4"/>
         <v>49</v>
@@ -4649,7 +4651,7 @@
         <v>53407170.701888472</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121">
         <f t="shared" si="4"/>
         <v>50</v>
@@ -4663,7 +4665,7 @@
         <v>52424999.806541555</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122">
         <f>A121+1</f>
         <v>51</v>
@@ -4677,7 +4679,7 @@
         <v>51460891.273513928</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123">
         <f t="shared" si="4"/>
         <v>52</v>
@@ -4691,7 +4693,7 @@
         <v>50514512.931557126</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124">
         <f t="shared" si="4"/>
         <v>53</v>
@@ -4705,7 +4707,7 @@
         <v>49585538.718132883</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125">
         <f t="shared" si="4"/>
         <v>54</v>
@@ -4719,7 +4721,7 @@
         <v>48673648.567072593</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126">
         <f t="shared" si="4"/>
         <v>55</v>
@@ -4733,7 +4735,7 @@
         <v>47778528.298302531</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127">
         <f t="shared" si="4"/>
         <v>56</v>
@@ -4747,7 +4749,7 @@
         <v>46899869.509597175</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128">
         <f t="shared" si="4"/>
         <v>57</v>
@@ -4761,7 +4763,7 @@
         <v>46037369.470323123</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129">
         <f>A128+1</f>
         <v>58</v>
@@ -4775,7 +4777,7 @@
         <v>45190731.017137192</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130">
         <f t="shared" si="4"/>
         <v>59</v>
@@ -4789,7 +4791,7 @@
         <v>44359662.451602511</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
         <f t="shared" si="4"/>
         <v>60</v>

</xml_diff>